<commit_message>
nmv 06 11 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 6.6 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 6.6 Padam Input Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6721BB-6A7F-4C8F-8A39-D9EB6917B8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943FB0FC-1EB7-4118-B2B0-CB584A7C7DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TS 6.6" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TS 6.6'!$C$1:$V$2126</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5485" uniqueCount="1316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5488" uniqueCount="1320">
   <si>
     <t>Passage</t>
   </si>
@@ -3972,17 +3972,41 @@
     <t>NE</t>
   </si>
   <si>
-    <t>yaqj~japaqtA(3),u</t>
-  </si>
-  <si>
     <t>anvanu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A and eti </t>
+  </si>
+  <si>
+    <t>yaqj~japaqtA(3)^^u</t>
+  </si>
+  <si>
+    <t>yaqj~japaqtA(3) viti</t>
+  </si>
+  <si>
+    <t>whether 2 maatas in anustaraNIm Gnanti??</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kampam, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>aBi cCandaH??</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4125,8 +4149,28 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4163,6 +4207,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -4191,7 +4247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4362,8 +4418,41 @@
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4645,12 +4734,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V2728"/>
+  <dimension ref="A1:V2126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2122" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="O19" sqref="O19"/>
+      <selection pane="bottomLeft" activeCell="N2127" sqref="N2127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -8038,7 +8127,9 @@
       <c r="V72" s="42"/>
     </row>
     <row r="73" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="8"/>
+      <c r="A73" s="8" t="s">
+        <v>1315</v>
+      </c>
       <c r="C73" s="10"/>
       <c r="D73" s="21"/>
       <c r="E73" s="10"/>
@@ -8065,7 +8156,7 @@
         <f t="shared" si="5"/>
         <v>72</v>
       </c>
-      <c r="N73" s="42" t="s">
+      <c r="N73" s="58" t="s">
         <v>112</v>
       </c>
       <c r="O73" s="8" t="s">
@@ -8103,7 +8194,7 @@
         <f t="shared" si="5"/>
         <v>73</v>
       </c>
-      <c r="N74" s="42" t="s">
+      <c r="N74" s="58" t="s">
         <v>181</v>
       </c>
       <c r="O74" s="7"/>
@@ -9459,7 +9550,7 @@
         <f t="shared" si="5"/>
         <v>110</v>
       </c>
-      <c r="N111" s="42" t="s">
+      <c r="N111" s="58" t="s">
         <v>112</v>
       </c>
       <c r="O111" s="8" t="s">
@@ -9503,7 +9594,7 @@
         <f t="shared" si="5"/>
         <v>111</v>
       </c>
-      <c r="N112" s="42" t="s">
+      <c r="N112" s="58" t="s">
         <v>151</v>
       </c>
       <c r="O112" s="8"/>
@@ -17420,7 +17511,9 @@
       <c r="V342" s="42"/>
     </row>
     <row r="343" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A343" s="8"/>
+      <c r="A343" s="60" t="s">
+        <v>1317</v>
+      </c>
       <c r="D343" s="22"/>
       <c r="F343" s="50" t="s">
         <v>129</v>
@@ -17446,8 +17539,8 @@
         <f t="shared" si="17"/>
         <v>104</v>
       </c>
-      <c r="N343" s="42" t="s">
-        <v>1314</v>
+      <c r="N343" s="60" t="s">
+        <v>1316</v>
       </c>
       <c r="O343" s="8" t="s">
         <v>64</v>
@@ -17486,7 +17579,7 @@
         <f t="shared" si="17"/>
         <v>105</v>
       </c>
-      <c r="N344" s="42" t="s">
+      <c r="N344" s="59" t="s">
         <v>169</v>
       </c>
       <c r="O344" s="7"/>
@@ -18760,7 +18853,7 @@
         <f t="shared" si="17"/>
         <v>141</v>
       </c>
-      <c r="N380" s="58" t="s">
+      <c r="N380" s="42" t="s">
         <v>325</v>
       </c>
       <c r="O380" s="8" t="s">
@@ -31088,37 +31181,37 @@
       <c r="V741" s="42"/>
     </row>
     <row r="742" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I742" s="45" t="s">
+      <c r="I742" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="J742" s="48">
+      <c r="J742" s="64">
         <v>15</v>
       </c>
-      <c r="K742" s="6">
+      <c r="K742" s="65">
         <f t="shared" si="33"/>
         <v>741</v>
       </c>
-      <c r="L742" s="6">
+      <c r="L742" s="65">
         <f t="shared" si="34"/>
         <v>50</v>
       </c>
-      <c r="M742" s="6">
+      <c r="M742" s="65">
         <f t="shared" si="35"/>
         <v>100</v>
       </c>
-      <c r="N742" s="42" t="s">
+      <c r="N742" s="61" t="s">
         <v>267</v>
       </c>
-      <c r="O742" s="8" t="s">
+      <c r="O742" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="P742" s="8"/>
-      <c r="Q742" s="8"/>
-      <c r="R742" s="8"/>
-      <c r="S742" s="8"/>
-      <c r="T742" s="8"/>
-      <c r="U742" s="8"/>
-      <c r="V742" s="42" t="s">
+      <c r="P742" s="62"/>
+      <c r="Q742" s="62"/>
+      <c r="R742" s="62"/>
+      <c r="S742" s="62"/>
+      <c r="T742" s="62"/>
+      <c r="U742" s="62"/>
+      <c r="V742" s="61" t="s">
         <v>1141</v>
       </c>
     </row>
@@ -37005,7 +37098,7 @@
         <f t="shared" si="44"/>
         <v>280</v>
       </c>
-      <c r="N922" s="58" t="s">
+      <c r="N922" s="42" t="s">
         <v>1289</v>
       </c>
       <c r="O922" s="8" t="s">
@@ -44116,7 +44209,7 @@
     </row>
     <row r="1142" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1142" s="8" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="I1142" s="45" t="s">
         <v>43</v>
@@ -46004,7 +46097,7 @@
       <c r="U1200" s="8"/>
       <c r="V1200" s="42"/>
     </row>
-    <row r="1201" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1201" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1201" s="45" t="s">
         <v>45</v>
       </c>
@@ -46039,7 +46132,7 @@
         <v>1187</v>
       </c>
     </row>
-    <row r="1202" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1202" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1202" s="45" t="s">
         <v>45</v>
       </c>
@@ -46070,7 +46163,7 @@
       <c r="U1202" s="8"/>
       <c r="V1202" s="42"/>
     </row>
-    <row r="1203" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1203" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1203" s="45" t="s">
         <v>45</v>
       </c>
@@ -46101,7 +46194,7 @@
       <c r="U1203" s="8"/>
       <c r="V1203" s="42"/>
     </row>
-    <row r="1204" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1204" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1204" s="45" t="s">
         <v>45</v>
       </c>
@@ -46132,7 +46225,7 @@
       <c r="U1204" s="8"/>
       <c r="V1204" s="42"/>
     </row>
-    <row r="1205" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1205" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1205" s="45" t="s">
         <v>45</v>
       </c>
@@ -46163,7 +46256,7 @@
       <c r="U1205" s="8"/>
       <c r="V1205" s="42"/>
     </row>
-    <row r="1206" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1206" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="G1206" s="50" t="s">
         <v>127</v>
       </c>
@@ -46197,7 +46290,14 @@
       <c r="U1206" s="8"/>
       <c r="V1206" s="42"/>
     </row>
-    <row r="1207" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1207" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A1207" s="67" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B1207" s="68"/>
+      <c r="C1207" s="51"/>
+      <c r="D1207" s="54"/>
+      <c r="E1207" s="51"/>
       <c r="G1207" s="50" t="s">
         <v>127</v>
       </c>
@@ -46219,7 +46319,7 @@
         <f t="shared" si="56"/>
         <v>12</v>
       </c>
-      <c r="N1207" s="42" t="s">
+      <c r="N1207" s="66" t="s">
         <v>698</v>
       </c>
       <c r="O1207" s="8" t="s">
@@ -46235,7 +46335,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="1208" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1208" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="G1208" s="50" t="s">
         <v>127</v>
       </c>
@@ -46257,7 +46357,7 @@
         <f t="shared" si="56"/>
         <v>13</v>
       </c>
-      <c r="N1208" s="42" t="s">
+      <c r="N1208" s="66" t="s">
         <v>692</v>
       </c>
       <c r="O1208" s="7"/>
@@ -46269,7 +46369,7 @@
       <c r="U1208" s="8"/>
       <c r="V1208" s="42"/>
     </row>
-    <row r="1209" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1209" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1209" s="45" t="s">
         <v>45</v>
       </c>
@@ -46300,7 +46400,7 @@
       <c r="U1209" s="8"/>
       <c r="V1209" s="42"/>
     </row>
-    <row r="1210" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1210" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1210" s="45" t="s">
         <v>45</v>
       </c>
@@ -46331,7 +46431,7 @@
       <c r="U1210" s="8"/>
       <c r="V1210" s="42"/>
     </row>
-    <row r="1211" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1211" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1211" s="45" t="s">
         <v>45</v>
       </c>
@@ -46362,7 +46462,7 @@
       <c r="U1211" s="8"/>
       <c r="V1211" s="42"/>
     </row>
-    <row r="1212" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1212" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1212" s="45" t="s">
         <v>45</v>
       </c>
@@ -46393,7 +46493,7 @@
       <c r="U1212" s="8"/>
       <c r="V1212" s="42"/>
     </row>
-    <row r="1213" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1213" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1213" s="45" t="s">
         <v>45</v>
       </c>
@@ -46428,7 +46528,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="1214" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1214" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1214" s="45" t="s">
         <v>45</v>
       </c>
@@ -46459,7 +46559,7 @@
       <c r="U1214" s="8"/>
       <c r="V1214" s="42"/>
     </row>
-    <row r="1215" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1215" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1215" s="45" t="s">
         <v>45</v>
       </c>
@@ -46490,7 +46590,7 @@
       <c r="U1215" s="8"/>
       <c r="V1215" s="42"/>
     </row>
-    <row r="1216" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1216" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1216" s="45" t="s">
         <v>45</v>
       </c>
@@ -61677,7 +61777,7 @@
         <f t="shared" si="80"/>
         <v>119</v>
       </c>
-      <c r="N1709" s="58" t="s">
+      <c r="N1709" s="42" t="s">
         <v>1292</v>
       </c>
       <c r="O1709" s="8" t="s">
@@ -70153,7 +70253,7 @@
         <f t="shared" si="95"/>
         <v>215</v>
       </c>
-      <c r="N2044" s="42" t="s">
+      <c r="N2044" s="66" t="s">
         <v>998</v>
       </c>
       <c r="S2044" s="1" t="s">
@@ -70165,8 +70265,8 @@
       <c r="V2044" s="42"/>
     </row>
     <row r="2045" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A2045" s="8" t="s">
-        <v>98</v>
+      <c r="A2045" s="69" t="s">
+        <v>1319</v>
       </c>
       <c r="H2045" s="49" t="s">
         <v>108</v>
@@ -70189,7 +70289,7 @@
         <f t="shared" si="95"/>
         <v>216</v>
       </c>
-      <c r="N2045" s="42" t="s">
+      <c r="N2045" s="66" t="s">
         <v>150</v>
       </c>
       <c r="O2045" s="7" t="s">
@@ -70521,7 +70621,7 @@
         <f t="shared" si="98"/>
         <v>229</v>
       </c>
-      <c r="N2058" s="42" t="s">
+      <c r="N2058" s="66" t="s">
         <v>998</v>
       </c>
       <c r="S2058" s="1" t="s">
@@ -70554,7 +70654,7 @@
         <f t="shared" si="98"/>
         <v>230</v>
       </c>
-      <c r="N2059" s="42" t="s">
+      <c r="N2059" s="66" t="s">
         <v>150</v>
       </c>
       <c r="O2059" s="7" t="s">
@@ -72283,3016 +72383,6 @@
       <c r="V2126" s="43" t="s">
         <v>1304</v>
       </c>
-    </row>
-    <row r="2127" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2127" s="45"/>
-      <c r="N2127" s="42"/>
-      <c r="V2127" s="42"/>
-    </row>
-    <row r="2128" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2128" s="45"/>
-      <c r="N2128" s="42"/>
-      <c r="V2128" s="42"/>
-    </row>
-    <row r="2129" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2129" s="45"/>
-      <c r="N2129" s="42"/>
-      <c r="V2129" s="42"/>
-    </row>
-    <row r="2130" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2130" s="45"/>
-      <c r="N2130" s="42"/>
-      <c r="V2130" s="42"/>
-    </row>
-    <row r="2131" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2131" s="45"/>
-      <c r="N2131" s="42"/>
-      <c r="V2131" s="42"/>
-    </row>
-    <row r="2132" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2132" s="45"/>
-      <c r="N2132" s="42"/>
-      <c r="V2132" s="42"/>
-    </row>
-    <row r="2133" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2133" s="45"/>
-      <c r="N2133" s="42"/>
-      <c r="V2133" s="42"/>
-    </row>
-    <row r="2134" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2134" s="45"/>
-      <c r="N2134" s="42"/>
-      <c r="V2134" s="42"/>
-    </row>
-    <row r="2135" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2135" s="45"/>
-      <c r="N2135" s="42"/>
-      <c r="V2135" s="42"/>
-    </row>
-    <row r="2136" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2136" s="45"/>
-      <c r="N2136" s="42"/>
-      <c r="V2136" s="42"/>
-    </row>
-    <row r="2137" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2137" s="45"/>
-      <c r="N2137" s="42"/>
-      <c r="V2137" s="42"/>
-    </row>
-    <row r="2138" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2138" s="45"/>
-      <c r="N2138" s="42"/>
-      <c r="V2138" s="42"/>
-    </row>
-    <row r="2139" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2139" s="45"/>
-      <c r="N2139" s="42"/>
-      <c r="V2139" s="42"/>
-    </row>
-    <row r="2140" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2140" s="45"/>
-      <c r="N2140" s="42"/>
-      <c r="V2140" s="42"/>
-    </row>
-    <row r="2141" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2141" s="45"/>
-      <c r="N2141" s="42"/>
-      <c r="V2141" s="42"/>
-    </row>
-    <row r="2142" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2142" s="45"/>
-      <c r="N2142" s="42"/>
-      <c r="V2142" s="42"/>
-    </row>
-    <row r="2143" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2143" s="45"/>
-      <c r="N2143" s="42"/>
-      <c r="V2143" s="42"/>
-    </row>
-    <row r="2144" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2144" s="45"/>
-      <c r="N2144" s="42"/>
-      <c r="V2144" s="42"/>
-    </row>
-    <row r="2145" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2145" s="45"/>
-      <c r="N2145" s="42"/>
-      <c r="V2145" s="42"/>
-    </row>
-    <row r="2146" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2146" s="45"/>
-      <c r="N2146" s="42"/>
-      <c r="V2146" s="42"/>
-    </row>
-    <row r="2147" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2147" s="45"/>
-      <c r="N2147" s="42"/>
-      <c r="V2147" s="42"/>
-    </row>
-    <row r="2148" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2148" s="45"/>
-      <c r="N2148" s="42"/>
-      <c r="V2148" s="42"/>
-    </row>
-    <row r="2149" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2149" s="45"/>
-      <c r="N2149" s="42"/>
-      <c r="V2149" s="42"/>
-    </row>
-    <row r="2150" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2150" s="45"/>
-      <c r="N2150" s="42"/>
-      <c r="V2150" s="42"/>
-    </row>
-    <row r="2151" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2151" s="45"/>
-      <c r="N2151" s="42"/>
-      <c r="V2151" s="42"/>
-    </row>
-    <row r="2152" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2152" s="45"/>
-      <c r="N2152" s="42"/>
-      <c r="V2152" s="42"/>
-    </row>
-    <row r="2153" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2153" s="45"/>
-      <c r="N2153" s="42"/>
-      <c r="V2153" s="42"/>
-    </row>
-    <row r="2154" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2154" s="45"/>
-      <c r="N2154" s="42"/>
-      <c r="V2154" s="42"/>
-    </row>
-    <row r="2155" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2155" s="45"/>
-      <c r="N2155" s="42"/>
-      <c r="V2155" s="42"/>
-    </row>
-    <row r="2156" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2156" s="45"/>
-      <c r="N2156" s="42"/>
-      <c r="V2156" s="42"/>
-    </row>
-    <row r="2157" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2157" s="45"/>
-      <c r="N2157" s="42"/>
-      <c r="V2157" s="42"/>
-    </row>
-    <row r="2158" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2158" s="45"/>
-      <c r="N2158" s="42"/>
-      <c r="V2158" s="42"/>
-    </row>
-    <row r="2159" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2159" s="45"/>
-      <c r="N2159" s="42"/>
-      <c r="V2159" s="42"/>
-    </row>
-    <row r="2160" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2160" s="45"/>
-      <c r="N2160" s="42"/>
-      <c r="V2160" s="42"/>
-    </row>
-    <row r="2161" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2161" s="45"/>
-      <c r="N2161" s="42"/>
-      <c r="V2161" s="42"/>
-    </row>
-    <row r="2162" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2162" s="45"/>
-      <c r="N2162" s="42"/>
-      <c r="V2162" s="42"/>
-    </row>
-    <row r="2163" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2163" s="45"/>
-      <c r="N2163" s="42"/>
-      <c r="V2163" s="42"/>
-    </row>
-    <row r="2164" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2164" s="45"/>
-      <c r="N2164" s="42"/>
-      <c r="V2164" s="42"/>
-    </row>
-    <row r="2165" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2165" s="45"/>
-      <c r="N2165" s="42"/>
-      <c r="V2165" s="42"/>
-    </row>
-    <row r="2166" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2166" s="45"/>
-      <c r="N2166" s="42"/>
-      <c r="V2166" s="42"/>
-    </row>
-    <row r="2167" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2167" s="45"/>
-      <c r="N2167" s="42"/>
-      <c r="V2167" s="42"/>
-    </row>
-    <row r="2168" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2168" s="45"/>
-      <c r="N2168" s="42"/>
-      <c r="V2168" s="42"/>
-    </row>
-    <row r="2169" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2169" s="45"/>
-      <c r="N2169" s="42"/>
-      <c r="V2169" s="42"/>
-    </row>
-    <row r="2170" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2170" s="45"/>
-      <c r="N2170" s="42"/>
-      <c r="V2170" s="42"/>
-    </row>
-    <row r="2171" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2171" s="45"/>
-      <c r="N2171" s="42"/>
-      <c r="V2171" s="42"/>
-    </row>
-    <row r="2172" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2172" s="45"/>
-      <c r="N2172" s="42"/>
-      <c r="V2172" s="42"/>
-    </row>
-    <row r="2173" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2173" s="45"/>
-      <c r="N2173" s="42"/>
-      <c r="V2173" s="42"/>
-    </row>
-    <row r="2174" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2174" s="45"/>
-      <c r="N2174" s="42"/>
-      <c r="V2174" s="42"/>
-    </row>
-    <row r="2175" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2175" s="45"/>
-      <c r="N2175" s="42"/>
-      <c r="V2175" s="42"/>
-    </row>
-    <row r="2176" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2176" s="45"/>
-      <c r="N2176" s="42"/>
-      <c r="V2176" s="42"/>
-    </row>
-    <row r="2177" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2177" s="45"/>
-      <c r="N2177" s="42"/>
-      <c r="V2177" s="42"/>
-    </row>
-    <row r="2178" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2178" s="45"/>
-      <c r="N2178" s="42"/>
-      <c r="V2178" s="42"/>
-    </row>
-    <row r="2179" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2179" s="45"/>
-      <c r="N2179" s="42"/>
-      <c r="V2179" s="42"/>
-    </row>
-    <row r="2180" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2180" s="45"/>
-      <c r="N2180" s="42"/>
-      <c r="V2180" s="42"/>
-    </row>
-    <row r="2181" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2181" s="45"/>
-      <c r="N2181" s="42"/>
-      <c r="V2181" s="42"/>
-    </row>
-    <row r="2182" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2182" s="45"/>
-      <c r="N2182" s="42"/>
-      <c r="V2182" s="42"/>
-    </row>
-    <row r="2183" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2183" s="45"/>
-      <c r="N2183" s="42"/>
-      <c r="V2183" s="42"/>
-    </row>
-    <row r="2184" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2184" s="45"/>
-      <c r="N2184" s="42"/>
-      <c r="V2184" s="42"/>
-    </row>
-    <row r="2185" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2185" s="45"/>
-      <c r="N2185" s="42"/>
-      <c r="V2185" s="42"/>
-    </row>
-    <row r="2186" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2186" s="45"/>
-      <c r="N2186" s="42"/>
-      <c r="V2186" s="42"/>
-    </row>
-    <row r="2187" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2187" s="45"/>
-      <c r="N2187" s="42"/>
-      <c r="V2187" s="42"/>
-    </row>
-    <row r="2188" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2188" s="45"/>
-      <c r="N2188" s="42"/>
-      <c r="V2188" s="42"/>
-    </row>
-    <row r="2189" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2189" s="45"/>
-      <c r="N2189" s="42"/>
-      <c r="V2189" s="42"/>
-    </row>
-    <row r="2190" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2190" s="45"/>
-      <c r="N2190" s="42"/>
-      <c r="V2190" s="42"/>
-    </row>
-    <row r="2191" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2191" s="45"/>
-      <c r="N2191" s="42"/>
-      <c r="V2191" s="42"/>
-    </row>
-    <row r="2192" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2192" s="45"/>
-      <c r="N2192" s="42"/>
-      <c r="V2192" s="42"/>
-    </row>
-    <row r="2193" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2193" s="45"/>
-      <c r="N2193" s="42"/>
-      <c r="V2193" s="42"/>
-    </row>
-    <row r="2194" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2194" s="45"/>
-      <c r="N2194" s="42"/>
-      <c r="V2194" s="42"/>
-    </row>
-    <row r="2195" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2195" s="45"/>
-      <c r="N2195" s="42"/>
-      <c r="V2195" s="42"/>
-    </row>
-    <row r="2196" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2196" s="45"/>
-      <c r="N2196" s="42"/>
-      <c r="V2196" s="42"/>
-    </row>
-    <row r="2197" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2197" s="45"/>
-      <c r="N2197" s="42"/>
-      <c r="V2197" s="42"/>
-    </row>
-    <row r="2198" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2198" s="45"/>
-      <c r="N2198" s="42"/>
-      <c r="V2198" s="42"/>
-    </row>
-    <row r="2199" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2199" s="45"/>
-      <c r="N2199" s="42"/>
-      <c r="V2199" s="42"/>
-    </row>
-    <row r="2200" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2200" s="45"/>
-      <c r="N2200" s="42"/>
-      <c r="V2200" s="42"/>
-    </row>
-    <row r="2201" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2201" s="45"/>
-      <c r="N2201" s="42"/>
-      <c r="V2201" s="42"/>
-    </row>
-    <row r="2202" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2202" s="45"/>
-      <c r="N2202" s="42"/>
-      <c r="V2202" s="42"/>
-    </row>
-    <row r="2203" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2203" s="45"/>
-      <c r="N2203" s="42"/>
-      <c r="V2203" s="42"/>
-    </row>
-    <row r="2204" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2204" s="45"/>
-      <c r="N2204" s="42"/>
-      <c r="V2204" s="42"/>
-    </row>
-    <row r="2205" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2205" s="45"/>
-      <c r="N2205" s="42"/>
-      <c r="V2205" s="42"/>
-    </row>
-    <row r="2206" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2206" s="45"/>
-      <c r="N2206" s="42"/>
-      <c r="V2206" s="42"/>
-    </row>
-    <row r="2207" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2207" s="45"/>
-      <c r="N2207" s="42"/>
-      <c r="V2207" s="42"/>
-    </row>
-    <row r="2208" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2208" s="45"/>
-      <c r="N2208" s="42"/>
-      <c r="V2208" s="42"/>
-    </row>
-    <row r="2209" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2209" s="45"/>
-      <c r="N2209" s="42"/>
-      <c r="V2209" s="42"/>
-    </row>
-    <row r="2210" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2210" s="45"/>
-      <c r="N2210" s="42"/>
-      <c r="V2210" s="42"/>
-    </row>
-    <row r="2211" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2211" s="45"/>
-      <c r="N2211" s="42"/>
-      <c r="V2211" s="42"/>
-    </row>
-    <row r="2212" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2212" s="45"/>
-      <c r="N2212" s="42"/>
-      <c r="V2212" s="42"/>
-    </row>
-    <row r="2213" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2213" s="45"/>
-      <c r="N2213" s="42"/>
-      <c r="V2213" s="42"/>
-    </row>
-    <row r="2214" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2214" s="45"/>
-      <c r="N2214" s="42"/>
-      <c r="V2214" s="42"/>
-    </row>
-    <row r="2215" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2215" s="45"/>
-      <c r="N2215" s="42"/>
-      <c r="V2215" s="42"/>
-    </row>
-    <row r="2216" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2216" s="45"/>
-      <c r="N2216" s="42"/>
-      <c r="V2216" s="42"/>
-    </row>
-    <row r="2217" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2217" s="45"/>
-      <c r="N2217" s="42"/>
-      <c r="V2217" s="42"/>
-    </row>
-    <row r="2218" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2218" s="45"/>
-      <c r="N2218" s="42"/>
-      <c r="V2218" s="42"/>
-    </row>
-    <row r="2219" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2219" s="45"/>
-      <c r="N2219" s="42"/>
-      <c r="V2219" s="42"/>
-    </row>
-    <row r="2220" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2220" s="45"/>
-      <c r="N2220" s="42"/>
-      <c r="V2220" s="42"/>
-    </row>
-    <row r="2221" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2221" s="45"/>
-      <c r="N2221" s="42"/>
-      <c r="V2221" s="42"/>
-    </row>
-    <row r="2222" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2222" s="45"/>
-      <c r="N2222" s="42"/>
-      <c r="V2222" s="42"/>
-    </row>
-    <row r="2223" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2223" s="45"/>
-      <c r="N2223" s="42"/>
-      <c r="V2223" s="42"/>
-    </row>
-    <row r="2224" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2224" s="45"/>
-      <c r="N2224" s="42"/>
-      <c r="V2224" s="42"/>
-    </row>
-    <row r="2225" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2225" s="45"/>
-      <c r="N2225" s="42"/>
-      <c r="V2225" s="42"/>
-    </row>
-    <row r="2226" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2226" s="45"/>
-      <c r="N2226" s="42"/>
-      <c r="V2226" s="42"/>
-    </row>
-    <row r="2227" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2227" s="45"/>
-      <c r="N2227" s="42"/>
-      <c r="V2227" s="42"/>
-    </row>
-    <row r="2228" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2228" s="45"/>
-      <c r="N2228" s="42"/>
-      <c r="V2228" s="42"/>
-    </row>
-    <row r="2229" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2229" s="45"/>
-      <c r="N2229" s="42"/>
-      <c r="V2229" s="42"/>
-    </row>
-    <row r="2230" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2230" s="45"/>
-      <c r="N2230" s="42"/>
-      <c r="V2230" s="42"/>
-    </row>
-    <row r="2231" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2231" s="45"/>
-      <c r="N2231" s="42"/>
-      <c r="V2231" s="42"/>
-    </row>
-    <row r="2232" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2232" s="45"/>
-      <c r="N2232" s="42"/>
-      <c r="V2232" s="42"/>
-    </row>
-    <row r="2233" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2233" s="45"/>
-      <c r="N2233" s="42"/>
-      <c r="V2233" s="42"/>
-    </row>
-    <row r="2234" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2234" s="45"/>
-      <c r="N2234" s="42"/>
-      <c r="V2234" s="42"/>
-    </row>
-    <row r="2235" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2235" s="45"/>
-      <c r="N2235" s="42"/>
-      <c r="V2235" s="42"/>
-    </row>
-    <row r="2236" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2236" s="45"/>
-      <c r="N2236" s="42"/>
-      <c r="V2236" s="42"/>
-    </row>
-    <row r="2237" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2237" s="45"/>
-      <c r="N2237" s="42"/>
-      <c r="V2237" s="42"/>
-    </row>
-    <row r="2238" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2238" s="45"/>
-      <c r="N2238" s="42"/>
-      <c r="V2238" s="42"/>
-    </row>
-    <row r="2239" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2239" s="45"/>
-      <c r="N2239" s="42"/>
-      <c r="V2239" s="42"/>
-    </row>
-    <row r="2240" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2240" s="45"/>
-      <c r="N2240" s="42"/>
-      <c r="V2240" s="42"/>
-    </row>
-    <row r="2241" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2241" s="45"/>
-      <c r="N2241" s="42"/>
-      <c r="V2241" s="42"/>
-    </row>
-    <row r="2242" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2242" s="45"/>
-      <c r="N2242" s="42"/>
-      <c r="V2242" s="42"/>
-    </row>
-    <row r="2243" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2243" s="45"/>
-      <c r="N2243" s="42"/>
-      <c r="V2243" s="42"/>
-    </row>
-    <row r="2244" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2244" s="45"/>
-      <c r="N2244" s="42"/>
-      <c r="V2244" s="42"/>
-    </row>
-    <row r="2245" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2245" s="45"/>
-      <c r="N2245" s="42"/>
-      <c r="V2245" s="42"/>
-    </row>
-    <row r="2246" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2246" s="45"/>
-      <c r="N2246" s="42"/>
-      <c r="V2246" s="42"/>
-    </row>
-    <row r="2247" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2247" s="45"/>
-      <c r="N2247" s="42"/>
-      <c r="V2247" s="42"/>
-    </row>
-    <row r="2248" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2248" s="45"/>
-      <c r="N2248" s="42"/>
-      <c r="V2248" s="42"/>
-    </row>
-    <row r="2249" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2249" s="45"/>
-      <c r="N2249" s="42"/>
-      <c r="V2249" s="42"/>
-    </row>
-    <row r="2250" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2250" s="45"/>
-      <c r="N2250" s="42"/>
-      <c r="V2250" s="42"/>
-    </row>
-    <row r="2251" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2251" s="45"/>
-      <c r="N2251" s="42"/>
-      <c r="V2251" s="42"/>
-    </row>
-    <row r="2252" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2252" s="45"/>
-      <c r="N2252" s="42"/>
-      <c r="V2252" s="42"/>
-    </row>
-    <row r="2253" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2253" s="45"/>
-      <c r="N2253" s="42"/>
-      <c r="V2253" s="42"/>
-    </row>
-    <row r="2254" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2254" s="45"/>
-      <c r="N2254" s="42"/>
-      <c r="V2254" s="42"/>
-    </row>
-    <row r="2255" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2255" s="45"/>
-      <c r="N2255" s="42"/>
-      <c r="V2255" s="42"/>
-    </row>
-    <row r="2256" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2256" s="45"/>
-      <c r="N2256" s="42"/>
-      <c r="V2256" s="42"/>
-    </row>
-    <row r="2257" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2257" s="45"/>
-      <c r="N2257" s="42"/>
-      <c r="V2257" s="42"/>
-    </row>
-    <row r="2258" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2258" s="45"/>
-      <c r="N2258" s="42"/>
-      <c r="V2258" s="42"/>
-    </row>
-    <row r="2259" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2259" s="45"/>
-      <c r="N2259" s="42"/>
-      <c r="V2259" s="42"/>
-    </row>
-    <row r="2260" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2260" s="45"/>
-      <c r="N2260" s="42"/>
-      <c r="V2260" s="42"/>
-    </row>
-    <row r="2261" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2261" s="45"/>
-      <c r="N2261" s="42"/>
-      <c r="V2261" s="42"/>
-    </row>
-    <row r="2262" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2262" s="45"/>
-      <c r="N2262" s="42"/>
-      <c r="V2262" s="42"/>
-    </row>
-    <row r="2263" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2263" s="45"/>
-      <c r="N2263" s="42"/>
-      <c r="V2263" s="42"/>
-    </row>
-    <row r="2264" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2264" s="45"/>
-      <c r="N2264" s="42"/>
-      <c r="V2264" s="42"/>
-    </row>
-    <row r="2265" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2265" s="45"/>
-      <c r="N2265" s="42"/>
-      <c r="V2265" s="42"/>
-    </row>
-    <row r="2266" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2266" s="45"/>
-      <c r="N2266" s="42"/>
-      <c r="V2266" s="42"/>
-    </row>
-    <row r="2267" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2267" s="45"/>
-      <c r="N2267" s="42"/>
-      <c r="V2267" s="42"/>
-    </row>
-    <row r="2268" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2268" s="45"/>
-      <c r="N2268" s="42"/>
-      <c r="V2268" s="42"/>
-    </row>
-    <row r="2269" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2269" s="45"/>
-      <c r="N2269" s="42"/>
-      <c r="V2269" s="42"/>
-    </row>
-    <row r="2270" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2270" s="45"/>
-      <c r="N2270" s="42"/>
-      <c r="V2270" s="42"/>
-    </row>
-    <row r="2271" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2271" s="45"/>
-      <c r="N2271" s="42"/>
-      <c r="V2271" s="42"/>
-    </row>
-    <row r="2272" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2272" s="45"/>
-      <c r="N2272" s="42"/>
-      <c r="V2272" s="42"/>
-    </row>
-    <row r="2273" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2273" s="45"/>
-      <c r="N2273" s="42"/>
-      <c r="V2273" s="42"/>
-    </row>
-    <row r="2274" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2274" s="45"/>
-      <c r="N2274" s="42"/>
-      <c r="V2274" s="42"/>
-    </row>
-    <row r="2275" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2275" s="45"/>
-      <c r="N2275" s="42"/>
-      <c r="V2275" s="42"/>
-    </row>
-    <row r="2276" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2276" s="45"/>
-      <c r="N2276" s="42"/>
-      <c r="V2276" s="42"/>
-    </row>
-    <row r="2277" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2277" s="45"/>
-      <c r="N2277" s="42"/>
-      <c r="V2277" s="42"/>
-    </row>
-    <row r="2278" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2278" s="45"/>
-      <c r="N2278" s="42"/>
-      <c r="V2278" s="42"/>
-    </row>
-    <row r="2279" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2279" s="45"/>
-      <c r="N2279" s="42"/>
-      <c r="V2279" s="42"/>
-    </row>
-    <row r="2280" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2280" s="45"/>
-      <c r="N2280" s="42"/>
-      <c r="V2280" s="42"/>
-    </row>
-    <row r="2281" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2281" s="45"/>
-      <c r="N2281" s="42"/>
-      <c r="V2281" s="42"/>
-    </row>
-    <row r="2282" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2282" s="45"/>
-      <c r="N2282" s="42"/>
-      <c r="V2282" s="42"/>
-    </row>
-    <row r="2283" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2283" s="45"/>
-      <c r="N2283" s="42"/>
-      <c r="V2283" s="42"/>
-    </row>
-    <row r="2284" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2284" s="45"/>
-      <c r="N2284" s="42"/>
-      <c r="V2284" s="42"/>
-    </row>
-    <row r="2285" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2285" s="45"/>
-      <c r="N2285" s="42"/>
-      <c r="V2285" s="42"/>
-    </row>
-    <row r="2286" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2286" s="45"/>
-      <c r="N2286" s="42"/>
-      <c r="V2286" s="42"/>
-    </row>
-    <row r="2287" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2287" s="45"/>
-      <c r="N2287" s="42"/>
-      <c r="V2287" s="42"/>
-    </row>
-    <row r="2288" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2288" s="45"/>
-      <c r="N2288" s="42"/>
-      <c r="V2288" s="42"/>
-    </row>
-    <row r="2289" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2289" s="45"/>
-      <c r="N2289" s="42"/>
-      <c r="V2289" s="42"/>
-    </row>
-    <row r="2290" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2290" s="45"/>
-      <c r="N2290" s="42"/>
-      <c r="V2290" s="42"/>
-    </row>
-    <row r="2291" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2291" s="45"/>
-      <c r="N2291" s="42"/>
-      <c r="V2291" s="42"/>
-    </row>
-    <row r="2292" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2292" s="45"/>
-      <c r="N2292" s="42"/>
-      <c r="V2292" s="42"/>
-    </row>
-    <row r="2293" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2293" s="45"/>
-      <c r="N2293" s="42"/>
-      <c r="V2293" s="42"/>
-    </row>
-    <row r="2294" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2294" s="45"/>
-      <c r="N2294" s="42"/>
-      <c r="V2294" s="42"/>
-    </row>
-    <row r="2295" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2295" s="45"/>
-      <c r="N2295" s="42"/>
-      <c r="V2295" s="42"/>
-    </row>
-    <row r="2296" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2296" s="45"/>
-      <c r="N2296" s="42"/>
-      <c r="V2296" s="42"/>
-    </row>
-    <row r="2297" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2297" s="45"/>
-      <c r="N2297" s="42"/>
-      <c r="V2297" s="42"/>
-    </row>
-    <row r="2298" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2298" s="45"/>
-      <c r="N2298" s="42"/>
-      <c r="V2298" s="42"/>
-    </row>
-    <row r="2299" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2299" s="45"/>
-      <c r="N2299" s="42"/>
-      <c r="V2299" s="42"/>
-    </row>
-    <row r="2300" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2300" s="45"/>
-      <c r="N2300" s="42"/>
-      <c r="V2300" s="42"/>
-    </row>
-    <row r="2301" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2301" s="45"/>
-      <c r="N2301" s="42"/>
-      <c r="V2301" s="42"/>
-    </row>
-    <row r="2302" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2302" s="45"/>
-      <c r="N2302" s="42"/>
-      <c r="V2302" s="42"/>
-    </row>
-    <row r="2303" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2303" s="45"/>
-      <c r="N2303" s="42"/>
-      <c r="V2303" s="42"/>
-    </row>
-    <row r="2304" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2304" s="45"/>
-      <c r="N2304" s="42"/>
-      <c r="V2304" s="42"/>
-    </row>
-    <row r="2305" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2305" s="45"/>
-      <c r="N2305" s="42"/>
-      <c r="V2305" s="42"/>
-    </row>
-    <row r="2306" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2306" s="45"/>
-      <c r="N2306" s="42"/>
-      <c r="V2306" s="42"/>
-    </row>
-    <row r="2307" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2307" s="45"/>
-      <c r="N2307" s="42"/>
-      <c r="V2307" s="42"/>
-    </row>
-    <row r="2308" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2308" s="45"/>
-      <c r="N2308" s="42"/>
-      <c r="V2308" s="42"/>
-    </row>
-    <row r="2309" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2309" s="45"/>
-      <c r="N2309" s="42"/>
-      <c r="V2309" s="42"/>
-    </row>
-    <row r="2310" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2310" s="45"/>
-      <c r="N2310" s="42"/>
-      <c r="V2310" s="42"/>
-    </row>
-    <row r="2311" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2311" s="45"/>
-      <c r="N2311" s="42"/>
-      <c r="V2311" s="42"/>
-    </row>
-    <row r="2312" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2312" s="45"/>
-      <c r="N2312" s="42"/>
-      <c r="V2312" s="42"/>
-    </row>
-    <row r="2313" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2313" s="45"/>
-      <c r="N2313" s="42"/>
-      <c r="V2313" s="42"/>
-    </row>
-    <row r="2314" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2314" s="45"/>
-      <c r="N2314" s="42"/>
-      <c r="V2314" s="42"/>
-    </row>
-    <row r="2315" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2315" s="45"/>
-      <c r="N2315" s="42"/>
-      <c r="V2315" s="42"/>
-    </row>
-    <row r="2316" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2316" s="45"/>
-      <c r="N2316" s="42"/>
-      <c r="V2316" s="42"/>
-    </row>
-    <row r="2317" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2317" s="45"/>
-      <c r="N2317" s="42"/>
-      <c r="V2317" s="42"/>
-    </row>
-    <row r="2318" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2318" s="45"/>
-      <c r="N2318" s="42"/>
-      <c r="V2318" s="42"/>
-    </row>
-    <row r="2319" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2319" s="45"/>
-      <c r="N2319" s="42"/>
-      <c r="V2319" s="42"/>
-    </row>
-    <row r="2320" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2320" s="45"/>
-      <c r="N2320" s="42"/>
-      <c r="V2320" s="42"/>
-    </row>
-    <row r="2321" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2321" s="45"/>
-      <c r="N2321" s="42"/>
-      <c r="V2321" s="42"/>
-    </row>
-    <row r="2322" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2322" s="45"/>
-      <c r="N2322" s="42"/>
-      <c r="V2322" s="42"/>
-    </row>
-    <row r="2323" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2323" s="45"/>
-      <c r="N2323" s="42"/>
-      <c r="V2323" s="42"/>
-    </row>
-    <row r="2324" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2324" s="45"/>
-      <c r="N2324" s="42"/>
-      <c r="V2324" s="42"/>
-    </row>
-    <row r="2325" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2325" s="45"/>
-      <c r="N2325" s="42"/>
-      <c r="V2325" s="42"/>
-    </row>
-    <row r="2326" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2326" s="45"/>
-      <c r="N2326" s="42"/>
-      <c r="V2326" s="42"/>
-    </row>
-    <row r="2327" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2327" s="45"/>
-      <c r="N2327" s="42"/>
-      <c r="V2327" s="42"/>
-    </row>
-    <row r="2328" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2328" s="45"/>
-      <c r="N2328" s="42"/>
-      <c r="V2328" s="42"/>
-    </row>
-    <row r="2329" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2329" s="45"/>
-      <c r="N2329" s="42"/>
-      <c r="V2329" s="42"/>
-    </row>
-    <row r="2330" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2330" s="45"/>
-      <c r="N2330" s="42"/>
-      <c r="V2330" s="42"/>
-    </row>
-    <row r="2331" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2331" s="45"/>
-      <c r="N2331" s="42"/>
-      <c r="V2331" s="42"/>
-    </row>
-    <row r="2332" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2332" s="45"/>
-      <c r="N2332" s="42"/>
-      <c r="V2332" s="42"/>
-    </row>
-    <row r="2333" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2333" s="45"/>
-      <c r="N2333" s="42"/>
-      <c r="V2333" s="42"/>
-    </row>
-    <row r="2334" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2334" s="45"/>
-      <c r="N2334" s="42"/>
-      <c r="V2334" s="42"/>
-    </row>
-    <row r="2335" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2335" s="45"/>
-      <c r="N2335" s="42"/>
-      <c r="V2335" s="42"/>
-    </row>
-    <row r="2336" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2336" s="45"/>
-      <c r="N2336" s="42"/>
-      <c r="V2336" s="42"/>
-    </row>
-    <row r="2337" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2337" s="45"/>
-      <c r="N2337" s="42"/>
-      <c r="V2337" s="42"/>
-    </row>
-    <row r="2338" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2338" s="45"/>
-      <c r="N2338" s="42"/>
-      <c r="V2338" s="42"/>
-    </row>
-    <row r="2339" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2339" s="45"/>
-      <c r="N2339" s="42"/>
-      <c r="V2339" s="42"/>
-    </row>
-    <row r="2340" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2340" s="45"/>
-      <c r="N2340" s="42"/>
-      <c r="V2340" s="42"/>
-    </row>
-    <row r="2341" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2341" s="45"/>
-      <c r="N2341" s="42"/>
-      <c r="V2341" s="42"/>
-    </row>
-    <row r="2342" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2342" s="45"/>
-      <c r="N2342" s="42"/>
-      <c r="V2342" s="42"/>
-    </row>
-    <row r="2343" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2343" s="45"/>
-      <c r="N2343" s="42"/>
-      <c r="V2343" s="42"/>
-    </row>
-    <row r="2344" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2344" s="45"/>
-      <c r="N2344" s="42"/>
-      <c r="V2344" s="42"/>
-    </row>
-    <row r="2345" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2345" s="45"/>
-      <c r="N2345" s="42"/>
-      <c r="V2345" s="42"/>
-    </row>
-    <row r="2346" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2346" s="45"/>
-      <c r="N2346" s="42"/>
-      <c r="V2346" s="42"/>
-    </row>
-    <row r="2347" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2347" s="45"/>
-      <c r="N2347" s="42"/>
-      <c r="V2347" s="42"/>
-    </row>
-    <row r="2348" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2348" s="45"/>
-      <c r="N2348" s="42"/>
-      <c r="V2348" s="42"/>
-    </row>
-    <row r="2349" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2349" s="45"/>
-      <c r="N2349" s="42"/>
-      <c r="V2349" s="42"/>
-    </row>
-    <row r="2350" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2350" s="45"/>
-      <c r="N2350" s="42"/>
-      <c r="V2350" s="42"/>
-    </row>
-    <row r="2351" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2351" s="45"/>
-      <c r="N2351" s="42"/>
-      <c r="V2351" s="42"/>
-    </row>
-    <row r="2352" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2352" s="45"/>
-      <c r="N2352" s="42"/>
-      <c r="V2352" s="42"/>
-    </row>
-    <row r="2353" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2353" s="45"/>
-      <c r="N2353" s="42"/>
-      <c r="V2353" s="42"/>
-    </row>
-    <row r="2354" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2354" s="45"/>
-      <c r="N2354" s="42"/>
-      <c r="V2354" s="42"/>
-    </row>
-    <row r="2355" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2355" s="45"/>
-      <c r="N2355" s="42"/>
-      <c r="V2355" s="42"/>
-    </row>
-    <row r="2356" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2356" s="45"/>
-      <c r="N2356" s="42"/>
-      <c r="V2356" s="42"/>
-    </row>
-    <row r="2357" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2357" s="45"/>
-      <c r="N2357" s="42"/>
-      <c r="V2357" s="42"/>
-    </row>
-    <row r="2358" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2358" s="45"/>
-      <c r="N2358" s="42"/>
-      <c r="V2358" s="42"/>
-    </row>
-    <row r="2359" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2359" s="45"/>
-      <c r="N2359" s="42"/>
-      <c r="V2359" s="42"/>
-    </row>
-    <row r="2360" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2360" s="45"/>
-      <c r="N2360" s="42"/>
-      <c r="V2360" s="42"/>
-    </row>
-    <row r="2361" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2361" s="45"/>
-      <c r="N2361" s="42"/>
-      <c r="V2361" s="42"/>
-    </row>
-    <row r="2362" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2362" s="45"/>
-      <c r="N2362" s="42"/>
-      <c r="V2362" s="42"/>
-    </row>
-    <row r="2363" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2363" s="45"/>
-      <c r="N2363" s="42"/>
-      <c r="V2363" s="42"/>
-    </row>
-    <row r="2364" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2364" s="45"/>
-      <c r="N2364" s="42"/>
-      <c r="V2364" s="42"/>
-    </row>
-    <row r="2365" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2365" s="45"/>
-      <c r="N2365" s="42"/>
-      <c r="V2365" s="42"/>
-    </row>
-    <row r="2366" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2366" s="45"/>
-      <c r="N2366" s="42"/>
-      <c r="V2366" s="42"/>
-    </row>
-    <row r="2367" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2367" s="45"/>
-      <c r="N2367" s="42"/>
-      <c r="V2367" s="42"/>
-    </row>
-    <row r="2368" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2368" s="45"/>
-      <c r="N2368" s="42"/>
-      <c r="V2368" s="42"/>
-    </row>
-    <row r="2369" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2369" s="45"/>
-      <c r="N2369" s="42"/>
-      <c r="V2369" s="42"/>
-    </row>
-    <row r="2370" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2370" s="45"/>
-      <c r="N2370" s="42"/>
-      <c r="V2370" s="42"/>
-    </row>
-    <row r="2371" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2371" s="45"/>
-      <c r="N2371" s="42"/>
-      <c r="V2371" s="42"/>
-    </row>
-    <row r="2372" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2372" s="45"/>
-      <c r="N2372" s="42"/>
-      <c r="V2372" s="42"/>
-    </row>
-    <row r="2373" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2373" s="45"/>
-      <c r="N2373" s="42"/>
-      <c r="V2373" s="42"/>
-    </row>
-    <row r="2374" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2374" s="45"/>
-      <c r="N2374" s="42"/>
-      <c r="V2374" s="42"/>
-    </row>
-    <row r="2375" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2375" s="45"/>
-      <c r="N2375" s="42"/>
-      <c r="V2375" s="42"/>
-    </row>
-    <row r="2376" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2376" s="45"/>
-      <c r="N2376" s="42"/>
-      <c r="V2376" s="42"/>
-    </row>
-    <row r="2377" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2377" s="45"/>
-      <c r="N2377" s="42"/>
-      <c r="V2377" s="42"/>
-    </row>
-    <row r="2378" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2378" s="45"/>
-      <c r="N2378" s="42"/>
-      <c r="V2378" s="42"/>
-    </row>
-    <row r="2379" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2379" s="45"/>
-      <c r="N2379" s="42"/>
-      <c r="V2379" s="42"/>
-    </row>
-    <row r="2380" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2380" s="45"/>
-      <c r="N2380" s="42"/>
-      <c r="V2380" s="42"/>
-    </row>
-    <row r="2381" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2381" s="45"/>
-      <c r="N2381" s="42"/>
-      <c r="V2381" s="42"/>
-    </row>
-    <row r="2382" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2382" s="45"/>
-      <c r="N2382" s="42"/>
-      <c r="V2382" s="42"/>
-    </row>
-    <row r="2383" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2383" s="45"/>
-      <c r="N2383" s="42"/>
-      <c r="V2383" s="42"/>
-    </row>
-    <row r="2384" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2384" s="45"/>
-      <c r="N2384" s="42"/>
-      <c r="V2384" s="42"/>
-    </row>
-    <row r="2385" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2385" s="45"/>
-      <c r="N2385" s="42"/>
-      <c r="V2385" s="42"/>
-    </row>
-    <row r="2386" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2386" s="45"/>
-      <c r="N2386" s="42"/>
-      <c r="V2386" s="42"/>
-    </row>
-    <row r="2387" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2387" s="45"/>
-      <c r="N2387" s="42"/>
-      <c r="V2387" s="42"/>
-    </row>
-    <row r="2388" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2388" s="45"/>
-      <c r="N2388" s="42"/>
-      <c r="V2388" s="42"/>
-    </row>
-    <row r="2389" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2389" s="45"/>
-      <c r="N2389" s="42"/>
-      <c r="V2389" s="42"/>
-    </row>
-    <row r="2390" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2390" s="45"/>
-      <c r="N2390" s="42"/>
-      <c r="V2390" s="42"/>
-    </row>
-    <row r="2391" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2391" s="45"/>
-      <c r="N2391" s="42"/>
-      <c r="V2391" s="42"/>
-    </row>
-    <row r="2392" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2392" s="45"/>
-      <c r="N2392" s="42"/>
-      <c r="V2392" s="42"/>
-    </row>
-    <row r="2393" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2393" s="45"/>
-      <c r="N2393" s="42"/>
-      <c r="V2393" s="42"/>
-    </row>
-    <row r="2394" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2394" s="45"/>
-      <c r="N2394" s="42"/>
-      <c r="V2394" s="42"/>
-    </row>
-    <row r="2395" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2395" s="45"/>
-      <c r="N2395" s="42"/>
-      <c r="V2395" s="42"/>
-    </row>
-    <row r="2396" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2396" s="45"/>
-      <c r="N2396" s="42"/>
-      <c r="V2396" s="42"/>
-    </row>
-    <row r="2397" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2397" s="45"/>
-      <c r="N2397" s="42"/>
-      <c r="V2397" s="42"/>
-    </row>
-    <row r="2398" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2398" s="45"/>
-      <c r="N2398" s="42"/>
-      <c r="V2398" s="42"/>
-    </row>
-    <row r="2399" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2399" s="45"/>
-      <c r="N2399" s="42"/>
-      <c r="V2399" s="42"/>
-    </row>
-    <row r="2400" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2400" s="45"/>
-      <c r="N2400" s="42"/>
-      <c r="V2400" s="42"/>
-    </row>
-    <row r="2401" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2401" s="45"/>
-      <c r="N2401" s="42"/>
-      <c r="V2401" s="42"/>
-    </row>
-    <row r="2402" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2402" s="45"/>
-      <c r="N2402" s="42"/>
-      <c r="V2402" s="42"/>
-    </row>
-    <row r="2403" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2403" s="45"/>
-      <c r="N2403" s="42"/>
-      <c r="V2403" s="42"/>
-    </row>
-    <row r="2404" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2404" s="45"/>
-      <c r="N2404" s="42"/>
-      <c r="V2404" s="42"/>
-    </row>
-    <row r="2405" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2405" s="45"/>
-      <c r="N2405" s="42"/>
-      <c r="V2405" s="42"/>
-    </row>
-    <row r="2406" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2406" s="45"/>
-      <c r="N2406" s="42"/>
-      <c r="V2406" s="42"/>
-    </row>
-    <row r="2407" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2407" s="45"/>
-      <c r="N2407" s="42"/>
-      <c r="V2407" s="42"/>
-    </row>
-    <row r="2408" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2408" s="45"/>
-      <c r="N2408" s="42"/>
-      <c r="V2408" s="42"/>
-    </row>
-    <row r="2409" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2409" s="45"/>
-      <c r="N2409" s="42"/>
-      <c r="V2409" s="42"/>
-    </row>
-    <row r="2410" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2410" s="45"/>
-      <c r="N2410" s="42"/>
-      <c r="V2410" s="42"/>
-    </row>
-    <row r="2411" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2411" s="45"/>
-      <c r="N2411" s="42"/>
-      <c r="V2411" s="42"/>
-    </row>
-    <row r="2412" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2412" s="45"/>
-      <c r="N2412" s="42"/>
-      <c r="V2412" s="42"/>
-    </row>
-    <row r="2413" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2413" s="45"/>
-      <c r="N2413" s="42"/>
-      <c r="V2413" s="42"/>
-    </row>
-    <row r="2414" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2414" s="45"/>
-      <c r="N2414" s="42"/>
-      <c r="V2414" s="42"/>
-    </row>
-    <row r="2415" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2415" s="45"/>
-      <c r="N2415" s="42"/>
-      <c r="V2415" s="42"/>
-    </row>
-    <row r="2416" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2416" s="45"/>
-      <c r="N2416" s="42"/>
-      <c r="V2416" s="42"/>
-    </row>
-    <row r="2417" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2417" s="45"/>
-      <c r="N2417" s="42"/>
-      <c r="V2417" s="42"/>
-    </row>
-    <row r="2418" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2418" s="45"/>
-      <c r="N2418" s="42"/>
-      <c r="V2418" s="42"/>
-    </row>
-    <row r="2419" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2419" s="45"/>
-      <c r="N2419" s="42"/>
-      <c r="V2419" s="42"/>
-    </row>
-    <row r="2420" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2420" s="45"/>
-      <c r="N2420" s="42"/>
-      <c r="V2420" s="42"/>
-    </row>
-    <row r="2421" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2421" s="45"/>
-      <c r="N2421" s="42"/>
-      <c r="V2421" s="42"/>
-    </row>
-    <row r="2422" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2422" s="45"/>
-      <c r="N2422" s="42"/>
-      <c r="V2422" s="42"/>
-    </row>
-    <row r="2423" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2423" s="45"/>
-      <c r="N2423" s="42"/>
-      <c r="V2423" s="42"/>
-    </row>
-    <row r="2424" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2424" s="45"/>
-      <c r="N2424" s="42"/>
-      <c r="V2424" s="42"/>
-    </row>
-    <row r="2425" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2425" s="45"/>
-      <c r="N2425" s="42"/>
-      <c r="V2425" s="42"/>
-    </row>
-    <row r="2426" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2426" s="45"/>
-      <c r="N2426" s="42"/>
-      <c r="V2426" s="42"/>
-    </row>
-    <row r="2427" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2427" s="45"/>
-      <c r="N2427" s="42"/>
-      <c r="V2427" s="42"/>
-    </row>
-    <row r="2428" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2428" s="45"/>
-      <c r="N2428" s="42"/>
-      <c r="V2428" s="42"/>
-    </row>
-    <row r="2429" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2429" s="45"/>
-      <c r="N2429" s="42"/>
-      <c r="V2429" s="42"/>
-    </row>
-    <row r="2430" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2430" s="45"/>
-      <c r="N2430" s="42"/>
-      <c r="V2430" s="42"/>
-    </row>
-    <row r="2431" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2431" s="45"/>
-      <c r="N2431" s="42"/>
-      <c r="V2431" s="42"/>
-    </row>
-    <row r="2432" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2432" s="45"/>
-      <c r="N2432" s="42"/>
-      <c r="V2432" s="42"/>
-    </row>
-    <row r="2433" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2433" s="45"/>
-      <c r="N2433" s="42"/>
-      <c r="V2433" s="42"/>
-    </row>
-    <row r="2434" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2434" s="45"/>
-      <c r="N2434" s="42"/>
-      <c r="V2434" s="42"/>
-    </row>
-    <row r="2435" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2435" s="45"/>
-      <c r="N2435" s="42"/>
-      <c r="V2435" s="42"/>
-    </row>
-    <row r="2436" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2436" s="45"/>
-      <c r="N2436" s="42"/>
-      <c r="V2436" s="42"/>
-    </row>
-    <row r="2437" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2437" s="45"/>
-      <c r="N2437" s="42"/>
-      <c r="V2437" s="42"/>
-    </row>
-    <row r="2438" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2438" s="45"/>
-      <c r="N2438" s="42"/>
-      <c r="V2438" s="42"/>
-    </row>
-    <row r="2439" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2439" s="45"/>
-      <c r="N2439" s="42"/>
-      <c r="V2439" s="42"/>
-    </row>
-    <row r="2440" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2440" s="45"/>
-      <c r="N2440" s="42"/>
-      <c r="V2440" s="42"/>
-    </row>
-    <row r="2441" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2441" s="45"/>
-      <c r="N2441" s="42"/>
-      <c r="V2441" s="42"/>
-    </row>
-    <row r="2442" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2442" s="45"/>
-      <c r="N2442" s="42"/>
-      <c r="V2442" s="42"/>
-    </row>
-    <row r="2443" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2443" s="45"/>
-      <c r="N2443" s="42"/>
-      <c r="V2443" s="42"/>
-    </row>
-    <row r="2444" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2444" s="45"/>
-      <c r="N2444" s="42"/>
-      <c r="V2444" s="42"/>
-    </row>
-    <row r="2445" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2445" s="45"/>
-      <c r="N2445" s="42"/>
-      <c r="V2445" s="42"/>
-    </row>
-    <row r="2446" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2446" s="45"/>
-      <c r="N2446" s="42"/>
-      <c r="V2446" s="42"/>
-    </row>
-    <row r="2447" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2447" s="45"/>
-      <c r="N2447" s="42"/>
-      <c r="V2447" s="42"/>
-    </row>
-    <row r="2448" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2448" s="45"/>
-      <c r="N2448" s="42"/>
-      <c r="V2448" s="42"/>
-    </row>
-    <row r="2449" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2449" s="45"/>
-      <c r="N2449" s="42"/>
-      <c r="V2449" s="42"/>
-    </row>
-    <row r="2450" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2450" s="45"/>
-      <c r="N2450" s="42"/>
-      <c r="V2450" s="42"/>
-    </row>
-    <row r="2451" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2451" s="45"/>
-      <c r="N2451" s="42"/>
-      <c r="V2451" s="42"/>
-    </row>
-    <row r="2452" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2452" s="45"/>
-      <c r="N2452" s="43"/>
-      <c r="V2452" s="43"/>
-    </row>
-    <row r="2453" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2453" s="45"/>
-      <c r="N2453" s="42"/>
-      <c r="V2453" s="42"/>
-    </row>
-    <row r="2454" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2454" s="45"/>
-      <c r="N2454" s="42"/>
-      <c r="V2454" s="42"/>
-    </row>
-    <row r="2455" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2455" s="45"/>
-      <c r="N2455" s="42"/>
-      <c r="V2455" s="42"/>
-    </row>
-    <row r="2456" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2456" s="45"/>
-      <c r="N2456" s="42"/>
-      <c r="V2456" s="42"/>
-    </row>
-    <row r="2457" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2457" s="45"/>
-      <c r="N2457" s="42"/>
-      <c r="V2457" s="42"/>
-    </row>
-    <row r="2458" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2458" s="45"/>
-      <c r="N2458" s="42"/>
-      <c r="V2458" s="42"/>
-    </row>
-    <row r="2459" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2459" s="45"/>
-      <c r="N2459" s="42"/>
-      <c r="V2459" s="42"/>
-    </row>
-    <row r="2460" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2460" s="45"/>
-      <c r="N2460" s="42"/>
-      <c r="V2460" s="42"/>
-    </row>
-    <row r="2461" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2461" s="45"/>
-      <c r="N2461" s="42"/>
-      <c r="V2461" s="42"/>
-    </row>
-    <row r="2462" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2462" s="45"/>
-      <c r="N2462" s="42"/>
-      <c r="V2462" s="42"/>
-    </row>
-    <row r="2463" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2463" s="45"/>
-      <c r="N2463" s="42"/>
-      <c r="V2463" s="42"/>
-    </row>
-    <row r="2464" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2464" s="45"/>
-      <c r="N2464" s="42"/>
-      <c r="V2464" s="42"/>
-    </row>
-    <row r="2465" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2465" s="45"/>
-      <c r="N2465" s="42"/>
-      <c r="V2465" s="42"/>
-    </row>
-    <row r="2466" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2466" s="45"/>
-      <c r="N2466" s="42"/>
-      <c r="V2466" s="42"/>
-    </row>
-    <row r="2467" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2467" s="45"/>
-      <c r="N2467" s="42"/>
-      <c r="V2467" s="42"/>
-    </row>
-    <row r="2468" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2468" s="45"/>
-      <c r="N2468" s="42"/>
-      <c r="V2468" s="42"/>
-    </row>
-    <row r="2469" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2469" s="45"/>
-      <c r="N2469" s="42"/>
-      <c r="V2469" s="42"/>
-    </row>
-    <row r="2470" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2470" s="45"/>
-      <c r="N2470" s="42"/>
-      <c r="V2470" s="42"/>
-    </row>
-    <row r="2471" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2471" s="45"/>
-      <c r="N2471" s="42"/>
-      <c r="V2471" s="42"/>
-    </row>
-    <row r="2472" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2472" s="45"/>
-      <c r="N2472" s="42"/>
-      <c r="V2472" s="42"/>
-    </row>
-    <row r="2473" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2473" s="45"/>
-      <c r="N2473" s="42"/>
-      <c r="V2473" s="42"/>
-    </row>
-    <row r="2474" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2474" s="45"/>
-      <c r="N2474" s="42"/>
-      <c r="V2474" s="42"/>
-    </row>
-    <row r="2475" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2475" s="45"/>
-      <c r="N2475" s="42"/>
-      <c r="V2475" s="42"/>
-    </row>
-    <row r="2476" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2476" s="45"/>
-      <c r="N2476" s="42"/>
-      <c r="V2476" s="42"/>
-    </row>
-    <row r="2477" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2477" s="45"/>
-      <c r="N2477" s="42"/>
-      <c r="V2477" s="42"/>
-    </row>
-    <row r="2478" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2478" s="45"/>
-      <c r="N2478" s="42"/>
-      <c r="V2478" s="42"/>
-    </row>
-    <row r="2479" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2479" s="45"/>
-      <c r="N2479" s="42"/>
-      <c r="V2479" s="42"/>
-    </row>
-    <row r="2480" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2480" s="45"/>
-      <c r="N2480" s="42"/>
-      <c r="V2480" s="42"/>
-    </row>
-    <row r="2481" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2481" s="45"/>
-      <c r="N2481" s="42"/>
-      <c r="V2481" s="42"/>
-    </row>
-    <row r="2482" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2482" s="45"/>
-      <c r="N2482" s="42"/>
-      <c r="V2482" s="42"/>
-    </row>
-    <row r="2483" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2483" s="45"/>
-      <c r="N2483" s="42"/>
-      <c r="V2483" s="42"/>
-    </row>
-    <row r="2484" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2484" s="45"/>
-      <c r="N2484" s="42"/>
-      <c r="V2484" s="42"/>
-    </row>
-    <row r="2485" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2485" s="45"/>
-      <c r="N2485" s="42"/>
-      <c r="V2485" s="42"/>
-    </row>
-    <row r="2486" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2486" s="45"/>
-      <c r="N2486" s="42"/>
-      <c r="V2486" s="42"/>
-    </row>
-    <row r="2487" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2487" s="45"/>
-      <c r="N2487" s="42"/>
-      <c r="V2487" s="42"/>
-    </row>
-    <row r="2488" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2488" s="45"/>
-      <c r="N2488" s="42"/>
-      <c r="V2488" s="42"/>
-    </row>
-    <row r="2489" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2489" s="45"/>
-      <c r="N2489" s="42"/>
-      <c r="V2489" s="42"/>
-    </row>
-    <row r="2490" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2490" s="45"/>
-      <c r="N2490" s="42"/>
-      <c r="V2490" s="42"/>
-    </row>
-    <row r="2491" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2491" s="45"/>
-      <c r="N2491" s="42"/>
-      <c r="V2491" s="42"/>
-    </row>
-    <row r="2492" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2492" s="45"/>
-      <c r="N2492" s="42"/>
-      <c r="V2492" s="42"/>
-    </row>
-    <row r="2493" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2493" s="45"/>
-      <c r="N2493" s="42"/>
-      <c r="V2493" s="42"/>
-    </row>
-    <row r="2494" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2494" s="45"/>
-      <c r="N2494" s="42"/>
-      <c r="V2494" s="42"/>
-    </row>
-    <row r="2495" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2495" s="45"/>
-      <c r="N2495" s="42"/>
-      <c r="V2495" s="42"/>
-    </row>
-    <row r="2496" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2496" s="45"/>
-      <c r="N2496" s="42"/>
-      <c r="V2496" s="42"/>
-    </row>
-    <row r="2497" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2497" s="45"/>
-      <c r="N2497" s="42"/>
-      <c r="V2497" s="42"/>
-    </row>
-    <row r="2498" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2498" s="45"/>
-      <c r="N2498" s="42"/>
-      <c r="V2498" s="42"/>
-    </row>
-    <row r="2499" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2499" s="45"/>
-      <c r="N2499" s="42"/>
-      <c r="V2499" s="42"/>
-    </row>
-    <row r="2500" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2500" s="45"/>
-      <c r="N2500" s="42"/>
-      <c r="V2500" s="42"/>
-    </row>
-    <row r="2501" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2501" s="45"/>
-      <c r="N2501" s="42"/>
-      <c r="V2501" s="42"/>
-    </row>
-    <row r="2502" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2502" s="45"/>
-      <c r="N2502" s="42"/>
-      <c r="V2502" s="42"/>
-    </row>
-    <row r="2503" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2503" s="45"/>
-      <c r="N2503" s="42"/>
-      <c r="V2503" s="42"/>
-    </row>
-    <row r="2504" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2504" s="45"/>
-      <c r="N2504" s="42"/>
-      <c r="V2504" s="42"/>
-    </row>
-    <row r="2505" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2505" s="45"/>
-      <c r="N2505" s="42"/>
-      <c r="V2505" s="42"/>
-    </row>
-    <row r="2506" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2506" s="45"/>
-      <c r="N2506" s="42"/>
-      <c r="V2506" s="42"/>
-    </row>
-    <row r="2507" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2507" s="45"/>
-      <c r="N2507" s="42"/>
-      <c r="V2507" s="42"/>
-    </row>
-    <row r="2508" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2508" s="45"/>
-      <c r="N2508" s="42"/>
-      <c r="V2508" s="42"/>
-    </row>
-    <row r="2509" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2509" s="45"/>
-      <c r="N2509" s="42"/>
-      <c r="V2509" s="42"/>
-    </row>
-    <row r="2510" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2510" s="45"/>
-      <c r="N2510" s="42"/>
-      <c r="V2510" s="42"/>
-    </row>
-    <row r="2511" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2511" s="45"/>
-      <c r="N2511" s="42"/>
-      <c r="V2511" s="42"/>
-    </row>
-    <row r="2512" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2512" s="45"/>
-      <c r="N2512" s="42"/>
-      <c r="V2512" s="42"/>
-    </row>
-    <row r="2513" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2513" s="45"/>
-      <c r="N2513" s="42"/>
-      <c r="V2513" s="42"/>
-    </row>
-    <row r="2514" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2514" s="45"/>
-      <c r="N2514" s="42"/>
-      <c r="V2514" s="42"/>
-    </row>
-    <row r="2515" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2515" s="45"/>
-      <c r="N2515" s="42"/>
-      <c r="V2515" s="42"/>
-    </row>
-    <row r="2516" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2516" s="45"/>
-      <c r="N2516" s="42"/>
-      <c r="V2516" s="42"/>
-    </row>
-    <row r="2517" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2517" s="45"/>
-      <c r="N2517" s="42"/>
-      <c r="V2517" s="42"/>
-    </row>
-    <row r="2518" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2518" s="45"/>
-      <c r="N2518" s="42"/>
-      <c r="V2518" s="42"/>
-    </row>
-    <row r="2519" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2519" s="45"/>
-      <c r="N2519" s="42"/>
-      <c r="V2519" s="42"/>
-    </row>
-    <row r="2520" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2520" s="45"/>
-      <c r="N2520" s="42"/>
-      <c r="V2520" s="42"/>
-    </row>
-    <row r="2521" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2521" s="45"/>
-      <c r="N2521" s="42"/>
-      <c r="V2521" s="42"/>
-    </row>
-    <row r="2522" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2522" s="45"/>
-      <c r="N2522" s="42"/>
-      <c r="V2522" s="42"/>
-    </row>
-    <row r="2523" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2523" s="45"/>
-      <c r="N2523" s="42"/>
-      <c r="V2523" s="42"/>
-    </row>
-    <row r="2524" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2524" s="45"/>
-      <c r="N2524" s="42"/>
-      <c r="V2524" s="42"/>
-    </row>
-    <row r="2525" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2525" s="45"/>
-      <c r="N2525" s="42"/>
-      <c r="V2525" s="42"/>
-    </row>
-    <row r="2526" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2526" s="45"/>
-      <c r="N2526" s="42"/>
-      <c r="V2526" s="42"/>
-    </row>
-    <row r="2527" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2527" s="45"/>
-      <c r="N2527" s="42"/>
-      <c r="V2527" s="42"/>
-    </row>
-    <row r="2528" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2528" s="45"/>
-      <c r="N2528" s="42"/>
-      <c r="V2528" s="42"/>
-    </row>
-    <row r="2529" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2529" s="45"/>
-      <c r="N2529" s="42"/>
-      <c r="V2529" s="42"/>
-    </row>
-    <row r="2530" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2530" s="45"/>
-      <c r="N2530" s="42"/>
-      <c r="V2530" s="42"/>
-    </row>
-    <row r="2531" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2531" s="45"/>
-      <c r="N2531" s="42"/>
-      <c r="V2531" s="42"/>
-    </row>
-    <row r="2532" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2532" s="45"/>
-      <c r="N2532" s="42"/>
-      <c r="V2532" s="42"/>
-    </row>
-    <row r="2533" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2533" s="45"/>
-      <c r="N2533" s="42"/>
-      <c r="V2533" s="42"/>
-    </row>
-    <row r="2534" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2534" s="45"/>
-      <c r="N2534" s="42"/>
-      <c r="V2534" s="42"/>
-    </row>
-    <row r="2535" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2535" s="45"/>
-      <c r="N2535" s="42"/>
-      <c r="V2535" s="42"/>
-    </row>
-    <row r="2536" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2536" s="45"/>
-      <c r="N2536" s="42"/>
-      <c r="V2536" s="42"/>
-    </row>
-    <row r="2537" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2537" s="45"/>
-      <c r="N2537" s="42"/>
-      <c r="V2537" s="42"/>
-    </row>
-    <row r="2538" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2538" s="45"/>
-      <c r="N2538" s="42"/>
-      <c r="V2538" s="42"/>
-    </row>
-    <row r="2539" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2539" s="45"/>
-      <c r="N2539" s="42"/>
-      <c r="V2539" s="42"/>
-    </row>
-    <row r="2540" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2540" s="45"/>
-      <c r="N2540" s="42"/>
-      <c r="V2540" s="42"/>
-    </row>
-    <row r="2541" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2541" s="45"/>
-      <c r="N2541" s="42"/>
-      <c r="V2541" s="42"/>
-    </row>
-    <row r="2542" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2542" s="45"/>
-      <c r="N2542" s="42"/>
-      <c r="V2542" s="42"/>
-    </row>
-    <row r="2543" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2543" s="45"/>
-      <c r="N2543" s="42"/>
-      <c r="V2543" s="42"/>
-    </row>
-    <row r="2544" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2544" s="45"/>
-      <c r="N2544" s="42"/>
-      <c r="V2544" s="42"/>
-    </row>
-    <row r="2545" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2545" s="45"/>
-      <c r="N2545" s="42"/>
-      <c r="V2545" s="42"/>
-    </row>
-    <row r="2546" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2546" s="45"/>
-      <c r="N2546" s="42"/>
-      <c r="V2546" s="42"/>
-    </row>
-    <row r="2547" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2547" s="45"/>
-      <c r="N2547" s="42"/>
-      <c r="V2547" s="42"/>
-    </row>
-    <row r="2548" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2548" s="45"/>
-      <c r="N2548" s="42"/>
-      <c r="V2548" s="42"/>
-    </row>
-    <row r="2549" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2549" s="45"/>
-      <c r="N2549" s="42"/>
-      <c r="V2549" s="42"/>
-    </row>
-    <row r="2550" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2550" s="45"/>
-      <c r="N2550" s="42"/>
-      <c r="V2550" s="42"/>
-    </row>
-    <row r="2551" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2551" s="45"/>
-      <c r="N2551" s="42"/>
-      <c r="V2551" s="42"/>
-    </row>
-    <row r="2552" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2552" s="45"/>
-      <c r="N2552" s="42"/>
-      <c r="V2552" s="42"/>
-    </row>
-    <row r="2553" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2553" s="45"/>
-      <c r="N2553" s="42"/>
-      <c r="V2553" s="42"/>
-    </row>
-    <row r="2554" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2554" s="45"/>
-      <c r="N2554" s="42"/>
-      <c r="V2554" s="42"/>
-    </row>
-    <row r="2555" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2555" s="45"/>
-      <c r="N2555" s="42"/>
-      <c r="V2555" s="42"/>
-    </row>
-    <row r="2556" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2556" s="45"/>
-      <c r="N2556" s="42"/>
-      <c r="V2556" s="42"/>
-    </row>
-    <row r="2557" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2557" s="45"/>
-      <c r="N2557" s="42"/>
-      <c r="V2557" s="42"/>
-    </row>
-    <row r="2558" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2558" s="45"/>
-      <c r="N2558" s="42"/>
-      <c r="V2558" s="42"/>
-    </row>
-    <row r="2559" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2559" s="45"/>
-      <c r="N2559" s="42"/>
-      <c r="V2559" s="42"/>
-    </row>
-    <row r="2560" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2560" s="45"/>
-      <c r="N2560" s="42"/>
-      <c r="V2560" s="42"/>
-    </row>
-    <row r="2561" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2561" s="45"/>
-      <c r="N2561" s="42"/>
-      <c r="V2561" s="42"/>
-    </row>
-    <row r="2562" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2562" s="45"/>
-      <c r="N2562" s="42"/>
-      <c r="V2562" s="42"/>
-    </row>
-    <row r="2563" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2563" s="45"/>
-      <c r="N2563" s="42"/>
-      <c r="V2563" s="42"/>
-    </row>
-    <row r="2564" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2564" s="45"/>
-      <c r="N2564" s="42"/>
-      <c r="V2564" s="42"/>
-    </row>
-    <row r="2565" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2565" s="45"/>
-      <c r="N2565" s="42"/>
-      <c r="V2565" s="42"/>
-    </row>
-    <row r="2566" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2566" s="45"/>
-      <c r="N2566" s="42"/>
-      <c r="V2566" s="42"/>
-    </row>
-    <row r="2567" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2567" s="45"/>
-      <c r="N2567" s="42"/>
-      <c r="V2567" s="42"/>
-    </row>
-    <row r="2568" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2568" s="45"/>
-      <c r="N2568" s="42"/>
-      <c r="V2568" s="42"/>
-    </row>
-    <row r="2569" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2569" s="45"/>
-      <c r="N2569" s="42"/>
-      <c r="V2569" s="42"/>
-    </row>
-    <row r="2570" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2570" s="45"/>
-      <c r="N2570" s="42"/>
-      <c r="V2570" s="42"/>
-    </row>
-    <row r="2571" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2571" s="45"/>
-      <c r="N2571" s="42"/>
-      <c r="V2571" s="42"/>
-    </row>
-    <row r="2572" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2572" s="45"/>
-      <c r="N2572" s="42"/>
-      <c r="V2572" s="42"/>
-    </row>
-    <row r="2573" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2573" s="45"/>
-      <c r="N2573" s="42"/>
-      <c r="V2573" s="42"/>
-    </row>
-    <row r="2574" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2574" s="45"/>
-      <c r="N2574" s="42"/>
-      <c r="V2574" s="42"/>
-    </row>
-    <row r="2575" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2575" s="45"/>
-      <c r="N2575" s="42"/>
-      <c r="V2575" s="42"/>
-    </row>
-    <row r="2576" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2576" s="45"/>
-      <c r="N2576" s="42"/>
-      <c r="V2576" s="42"/>
-    </row>
-    <row r="2577" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2577" s="45"/>
-      <c r="N2577" s="42"/>
-      <c r="V2577" s="42"/>
-    </row>
-    <row r="2578" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2578" s="45"/>
-      <c r="N2578" s="42"/>
-      <c r="V2578" s="42"/>
-    </row>
-    <row r="2579" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2579" s="45"/>
-      <c r="N2579" s="42"/>
-      <c r="V2579" s="42"/>
-    </row>
-    <row r="2580" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2580" s="45"/>
-      <c r="N2580" s="42"/>
-      <c r="V2580" s="42"/>
-    </row>
-    <row r="2581" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2581" s="45"/>
-      <c r="N2581" s="42"/>
-      <c r="V2581" s="42"/>
-    </row>
-    <row r="2582" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2582" s="45"/>
-      <c r="N2582" s="42"/>
-      <c r="V2582" s="42"/>
-    </row>
-    <row r="2583" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2583" s="45"/>
-      <c r="N2583" s="42"/>
-      <c r="V2583" s="42"/>
-    </row>
-    <row r="2584" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2584" s="45"/>
-      <c r="N2584" s="42"/>
-      <c r="V2584" s="42"/>
-    </row>
-    <row r="2585" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2585" s="45"/>
-      <c r="N2585" s="42"/>
-      <c r="V2585" s="42"/>
-    </row>
-    <row r="2586" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2586" s="45"/>
-      <c r="N2586" s="42"/>
-      <c r="V2586" s="42"/>
-    </row>
-    <row r="2587" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2587" s="45"/>
-      <c r="N2587" s="42"/>
-      <c r="V2587" s="42"/>
-    </row>
-    <row r="2588" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2588" s="45"/>
-      <c r="N2588" s="42"/>
-      <c r="V2588" s="42"/>
-    </row>
-    <row r="2589" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2589" s="45"/>
-      <c r="N2589" s="42"/>
-      <c r="V2589" s="42"/>
-    </row>
-    <row r="2590" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2590" s="45"/>
-      <c r="N2590" s="42"/>
-      <c r="V2590" s="42"/>
-    </row>
-    <row r="2591" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2591" s="45"/>
-      <c r="N2591" s="42"/>
-      <c r="V2591" s="42"/>
-    </row>
-    <row r="2592" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2592" s="45"/>
-      <c r="N2592" s="42"/>
-      <c r="V2592" s="42"/>
-    </row>
-    <row r="2593" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2593" s="45"/>
-      <c r="N2593" s="42"/>
-      <c r="V2593" s="42"/>
-    </row>
-    <row r="2594" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2594" s="45"/>
-      <c r="N2594" s="42"/>
-      <c r="V2594" s="42"/>
-    </row>
-    <row r="2595" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2595" s="45"/>
-      <c r="N2595" s="42"/>
-      <c r="V2595" s="42"/>
-    </row>
-    <row r="2596" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2596" s="45"/>
-      <c r="N2596" s="42"/>
-      <c r="V2596" s="42"/>
-    </row>
-    <row r="2597" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2597" s="45"/>
-      <c r="N2597" s="42"/>
-      <c r="V2597" s="42"/>
-    </row>
-    <row r="2598" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2598" s="45"/>
-      <c r="N2598" s="42"/>
-      <c r="V2598" s="42"/>
-    </row>
-    <row r="2599" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2599" s="45"/>
-      <c r="N2599" s="42"/>
-      <c r="V2599" s="42"/>
-    </row>
-    <row r="2600" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2600" s="45"/>
-      <c r="N2600" s="42"/>
-      <c r="V2600" s="42"/>
-    </row>
-    <row r="2601" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2601" s="45"/>
-      <c r="N2601" s="42"/>
-      <c r="V2601" s="42"/>
-    </row>
-    <row r="2602" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2602" s="45"/>
-      <c r="N2602" s="42"/>
-      <c r="V2602" s="42"/>
-    </row>
-    <row r="2603" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2603" s="45"/>
-      <c r="N2603" s="42"/>
-      <c r="V2603" s="42"/>
-    </row>
-    <row r="2604" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2604" s="45"/>
-      <c r="N2604" s="42"/>
-      <c r="V2604" s="42"/>
-    </row>
-    <row r="2605" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2605" s="45"/>
-      <c r="N2605" s="42"/>
-      <c r="V2605" s="42"/>
-    </row>
-    <row r="2606" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2606" s="45"/>
-      <c r="N2606" s="42"/>
-      <c r="V2606" s="42"/>
-    </row>
-    <row r="2607" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2607" s="45"/>
-      <c r="N2607" s="42"/>
-      <c r="V2607" s="42"/>
-    </row>
-    <row r="2608" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2608" s="45"/>
-      <c r="N2608" s="42"/>
-      <c r="V2608" s="42"/>
-    </row>
-    <row r="2609" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2609" s="45"/>
-      <c r="N2609" s="42"/>
-      <c r="V2609" s="42"/>
-    </row>
-    <row r="2610" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2610" s="45"/>
-      <c r="N2610" s="42"/>
-      <c r="V2610" s="42"/>
-    </row>
-    <row r="2611" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2611" s="45"/>
-      <c r="N2611" s="42"/>
-      <c r="V2611" s="42"/>
-    </row>
-    <row r="2612" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2612" s="45"/>
-      <c r="N2612" s="42"/>
-      <c r="V2612" s="42"/>
-    </row>
-    <row r="2613" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2613" s="45"/>
-      <c r="N2613" s="42"/>
-      <c r="V2613" s="42"/>
-    </row>
-    <row r="2614" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2614" s="45"/>
-      <c r="N2614" s="42"/>
-      <c r="V2614" s="42"/>
-    </row>
-    <row r="2615" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2615" s="45"/>
-      <c r="N2615" s="42"/>
-      <c r="V2615" s="42"/>
-    </row>
-    <row r="2616" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2616" s="45"/>
-      <c r="N2616" s="42"/>
-      <c r="V2616" s="42"/>
-    </row>
-    <row r="2617" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2617" s="45"/>
-      <c r="N2617" s="42"/>
-      <c r="V2617" s="42"/>
-    </row>
-    <row r="2618" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2618" s="45"/>
-      <c r="N2618" s="42"/>
-      <c r="V2618" s="42"/>
-    </row>
-    <row r="2619" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2619" s="45"/>
-      <c r="N2619" s="42"/>
-      <c r="V2619" s="42"/>
-    </row>
-    <row r="2620" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2620" s="45"/>
-      <c r="N2620" s="42"/>
-      <c r="V2620" s="42"/>
-    </row>
-    <row r="2621" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2621" s="45"/>
-      <c r="N2621" s="42"/>
-      <c r="V2621" s="42"/>
-    </row>
-    <row r="2622" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2622" s="45"/>
-      <c r="N2622" s="42"/>
-      <c r="V2622" s="42"/>
-    </row>
-    <row r="2623" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2623" s="45"/>
-      <c r="N2623" s="42"/>
-      <c r="V2623" s="42"/>
-    </row>
-    <row r="2624" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2624" s="45"/>
-      <c r="N2624" s="42"/>
-      <c r="V2624" s="42"/>
-    </row>
-    <row r="2625" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2625" s="45"/>
-      <c r="N2625" s="42"/>
-      <c r="V2625" s="42"/>
-    </row>
-    <row r="2626" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2626" s="45"/>
-      <c r="N2626" s="42"/>
-      <c r="V2626" s="42"/>
-    </row>
-    <row r="2627" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2627" s="45"/>
-      <c r="N2627" s="42"/>
-      <c r="V2627" s="42"/>
-    </row>
-    <row r="2628" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2628" s="45"/>
-      <c r="N2628" s="42"/>
-      <c r="V2628" s="42"/>
-    </row>
-    <row r="2629" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2629" s="45"/>
-      <c r="N2629" s="42"/>
-      <c r="V2629" s="42"/>
-    </row>
-    <row r="2630" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2630" s="45"/>
-      <c r="N2630" s="42"/>
-      <c r="V2630" s="42"/>
-    </row>
-    <row r="2631" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2631" s="45"/>
-      <c r="N2631" s="42"/>
-      <c r="V2631" s="42"/>
-    </row>
-    <row r="2632" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2632" s="45"/>
-      <c r="N2632" s="42"/>
-      <c r="V2632" s="42"/>
-    </row>
-    <row r="2633" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2633" s="45"/>
-      <c r="N2633" s="42"/>
-      <c r="V2633" s="42"/>
-    </row>
-    <row r="2634" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2634" s="45"/>
-      <c r="N2634" s="42"/>
-      <c r="V2634" s="42"/>
-    </row>
-    <row r="2635" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2635" s="45"/>
-      <c r="N2635" s="42"/>
-      <c r="V2635" s="42"/>
-    </row>
-    <row r="2636" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2636" s="45"/>
-      <c r="N2636" s="42"/>
-      <c r="V2636" s="42"/>
-    </row>
-    <row r="2637" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2637" s="45"/>
-      <c r="N2637" s="42"/>
-      <c r="V2637" s="42"/>
-    </row>
-    <row r="2638" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2638" s="45"/>
-      <c r="N2638" s="42"/>
-      <c r="V2638" s="42"/>
-    </row>
-    <row r="2639" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2639" s="45"/>
-      <c r="N2639" s="42"/>
-      <c r="V2639" s="42"/>
-    </row>
-    <row r="2640" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2640" s="45"/>
-      <c r="N2640" s="42"/>
-      <c r="V2640" s="42"/>
-    </row>
-    <row r="2641" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2641" s="45"/>
-      <c r="N2641" s="42"/>
-      <c r="V2641" s="42"/>
-    </row>
-    <row r="2642" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2642" s="45"/>
-      <c r="N2642" s="42"/>
-      <c r="V2642" s="42"/>
-    </row>
-    <row r="2643" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2643" s="45"/>
-      <c r="N2643" s="42"/>
-      <c r="V2643" s="42"/>
-    </row>
-    <row r="2644" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2644" s="45"/>
-      <c r="N2644" s="42"/>
-      <c r="V2644" s="42"/>
-    </row>
-    <row r="2645" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2645" s="45"/>
-      <c r="N2645" s="42"/>
-      <c r="V2645" s="42"/>
-    </row>
-    <row r="2646" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2646" s="45"/>
-      <c r="N2646" s="42"/>
-      <c r="V2646" s="42"/>
-    </row>
-    <row r="2647" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2647" s="45"/>
-      <c r="N2647" s="42"/>
-      <c r="V2647" s="42"/>
-    </row>
-    <row r="2648" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2648" s="45"/>
-      <c r="N2648" s="42"/>
-      <c r="V2648" s="42"/>
-    </row>
-    <row r="2649" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2649" s="45"/>
-      <c r="N2649" s="42"/>
-      <c r="V2649" s="42"/>
-    </row>
-    <row r="2650" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2650" s="45"/>
-      <c r="N2650" s="42"/>
-      <c r="V2650" s="42"/>
-    </row>
-    <row r="2651" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2651" s="45"/>
-      <c r="N2651" s="42"/>
-      <c r="V2651" s="42"/>
-    </row>
-    <row r="2652" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2652" s="45"/>
-      <c r="N2652" s="42"/>
-      <c r="V2652" s="42"/>
-    </row>
-    <row r="2653" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2653" s="45"/>
-      <c r="N2653" s="42"/>
-      <c r="V2653" s="42"/>
-    </row>
-    <row r="2654" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2654" s="45"/>
-      <c r="N2654" s="42"/>
-      <c r="V2654" s="42"/>
-    </row>
-    <row r="2655" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2655" s="45"/>
-      <c r="N2655" s="42"/>
-      <c r="V2655" s="42"/>
-    </row>
-    <row r="2656" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2656" s="45"/>
-      <c r="N2656" s="42"/>
-      <c r="V2656" s="42"/>
-    </row>
-    <row r="2657" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2657" s="45"/>
-      <c r="N2657" s="42"/>
-      <c r="V2657" s="42"/>
-    </row>
-    <row r="2658" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2658" s="45"/>
-      <c r="N2658" s="42"/>
-      <c r="V2658" s="42"/>
-    </row>
-    <row r="2659" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2659" s="45"/>
-      <c r="N2659" s="42"/>
-      <c r="V2659" s="42"/>
-    </row>
-    <row r="2660" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2660" s="45"/>
-      <c r="N2660" s="42"/>
-      <c r="V2660" s="42"/>
-    </row>
-    <row r="2661" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2661" s="45"/>
-      <c r="N2661" s="42"/>
-      <c r="V2661" s="42"/>
-    </row>
-    <row r="2662" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2662" s="45"/>
-      <c r="N2662" s="42"/>
-      <c r="V2662" s="42"/>
-    </row>
-    <row r="2663" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2663" s="45"/>
-      <c r="N2663" s="42"/>
-      <c r="V2663" s="42"/>
-    </row>
-    <row r="2664" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2664" s="45"/>
-      <c r="N2664" s="42"/>
-      <c r="V2664" s="42"/>
-    </row>
-    <row r="2665" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2665" s="45"/>
-      <c r="N2665" s="42"/>
-      <c r="V2665" s="42"/>
-    </row>
-    <row r="2666" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2666" s="45"/>
-      <c r="N2666" s="42"/>
-      <c r="V2666" s="42"/>
-    </row>
-    <row r="2667" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2667" s="45"/>
-      <c r="N2667" s="42"/>
-      <c r="V2667" s="42"/>
-    </row>
-    <row r="2668" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2668" s="45"/>
-      <c r="N2668" s="42"/>
-      <c r="V2668" s="42"/>
-    </row>
-    <row r="2669" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2669" s="45"/>
-      <c r="N2669" s="42"/>
-      <c r="V2669" s="42"/>
-    </row>
-    <row r="2670" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2670" s="45"/>
-      <c r="N2670" s="42"/>
-      <c r="V2670" s="42"/>
-    </row>
-    <row r="2671" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2671" s="45"/>
-      <c r="N2671" s="42"/>
-      <c r="V2671" s="42"/>
-    </row>
-    <row r="2672" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2672" s="45"/>
-      <c r="N2672" s="42"/>
-      <c r="V2672" s="42"/>
-    </row>
-    <row r="2673" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2673" s="45"/>
-      <c r="N2673" s="42"/>
-      <c r="V2673" s="42"/>
-    </row>
-    <row r="2674" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2674" s="45"/>
-      <c r="N2674" s="42"/>
-      <c r="V2674" s="42"/>
-    </row>
-    <row r="2675" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2675" s="45"/>
-      <c r="N2675" s="42"/>
-      <c r="V2675" s="42"/>
-    </row>
-    <row r="2676" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2676" s="45"/>
-      <c r="N2676" s="42"/>
-      <c r="V2676" s="42"/>
-    </row>
-    <row r="2677" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2677" s="45"/>
-      <c r="N2677" s="42"/>
-      <c r="V2677" s="42"/>
-    </row>
-    <row r="2678" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2678" s="45"/>
-      <c r="N2678" s="42"/>
-      <c r="V2678" s="42"/>
-    </row>
-    <row r="2679" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2679" s="45"/>
-      <c r="N2679" s="42"/>
-      <c r="V2679" s="42"/>
-    </row>
-    <row r="2680" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2680" s="45"/>
-      <c r="N2680" s="42"/>
-      <c r="V2680" s="42"/>
-    </row>
-    <row r="2681" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2681" s="45"/>
-      <c r="N2681" s="42"/>
-      <c r="V2681" s="42"/>
-    </row>
-    <row r="2682" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2682" s="45"/>
-      <c r="N2682" s="42"/>
-      <c r="V2682" s="42"/>
-    </row>
-    <row r="2683" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2683" s="45"/>
-      <c r="N2683" s="42"/>
-      <c r="V2683" s="42"/>
-    </row>
-    <row r="2684" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2684" s="45"/>
-      <c r="N2684" s="42"/>
-      <c r="V2684" s="42"/>
-    </row>
-    <row r="2685" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2685" s="45"/>
-      <c r="N2685" s="42"/>
-      <c r="V2685" s="42"/>
-    </row>
-    <row r="2686" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2686" s="45"/>
-      <c r="N2686" s="42"/>
-      <c r="V2686" s="42"/>
-    </row>
-    <row r="2687" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2687" s="45"/>
-      <c r="N2687" s="42"/>
-      <c r="V2687" s="42"/>
-    </row>
-    <row r="2688" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2688" s="45"/>
-      <c r="N2688" s="42"/>
-      <c r="V2688" s="42"/>
-    </row>
-    <row r="2689" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2689" s="45"/>
-      <c r="N2689" s="42"/>
-      <c r="V2689" s="42"/>
-    </row>
-    <row r="2690" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2690" s="45"/>
-      <c r="N2690" s="42"/>
-      <c r="V2690" s="42"/>
-    </row>
-    <row r="2691" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2691" s="45"/>
-      <c r="N2691" s="42"/>
-      <c r="V2691" s="42"/>
-    </row>
-    <row r="2692" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2692" s="45"/>
-      <c r="N2692" s="42"/>
-      <c r="V2692" s="42"/>
-    </row>
-    <row r="2693" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2693" s="45"/>
-      <c r="N2693" s="42"/>
-      <c r="V2693" s="42"/>
-    </row>
-    <row r="2694" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2694" s="45"/>
-      <c r="N2694" s="42"/>
-      <c r="V2694" s="42"/>
-    </row>
-    <row r="2695" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2695" s="45"/>
-      <c r="N2695" s="42"/>
-      <c r="V2695" s="42"/>
-    </row>
-    <row r="2696" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2696" s="45"/>
-      <c r="N2696" s="42"/>
-      <c r="V2696" s="42"/>
-    </row>
-    <row r="2697" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2697" s="45"/>
-      <c r="N2697" s="42"/>
-      <c r="V2697" s="42"/>
-    </row>
-    <row r="2698" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2698" s="45"/>
-      <c r="N2698" s="42"/>
-      <c r="V2698" s="42"/>
-    </row>
-    <row r="2699" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2699" s="45"/>
-      <c r="N2699" s="42"/>
-      <c r="V2699" s="42"/>
-    </row>
-    <row r="2700" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2700" s="45"/>
-      <c r="N2700" s="42"/>
-      <c r="V2700" s="42"/>
-    </row>
-    <row r="2701" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2701" s="45"/>
-      <c r="N2701" s="42"/>
-      <c r="V2701" s="42"/>
-    </row>
-    <row r="2702" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2702" s="45"/>
-      <c r="N2702" s="42"/>
-      <c r="V2702" s="42"/>
-    </row>
-    <row r="2703" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2703" s="45"/>
-      <c r="N2703" s="42"/>
-      <c r="V2703" s="42"/>
-    </row>
-    <row r="2704" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2704" s="45"/>
-      <c r="N2704" s="42"/>
-      <c r="V2704" s="42"/>
-    </row>
-    <row r="2705" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2705" s="45"/>
-      <c r="N2705" s="42"/>
-      <c r="V2705" s="42"/>
-    </row>
-    <row r="2706" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2706" s="45"/>
-      <c r="N2706" s="42"/>
-      <c r="V2706" s="42"/>
-    </row>
-    <row r="2707" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2707" s="45"/>
-      <c r="N2707" s="42"/>
-      <c r="V2707" s="42"/>
-    </row>
-    <row r="2708" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2708" s="45"/>
-      <c r="N2708" s="42"/>
-      <c r="V2708" s="42"/>
-    </row>
-    <row r="2709" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2709" s="45"/>
-      <c r="N2709" s="42"/>
-      <c r="V2709" s="42"/>
-    </row>
-    <row r="2710" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2710" s="45"/>
-      <c r="N2710" s="42"/>
-      <c r="V2710" s="42"/>
-    </row>
-    <row r="2711" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2711" s="45"/>
-      <c r="N2711" s="42"/>
-      <c r="V2711" s="42"/>
-    </row>
-    <row r="2712" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2712" s="45"/>
-      <c r="N2712" s="42"/>
-      <c r="V2712" s="42"/>
-    </row>
-    <row r="2713" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2713" s="45"/>
-      <c r="N2713" s="42"/>
-      <c r="V2713" s="42"/>
-    </row>
-    <row r="2714" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2714" s="45"/>
-      <c r="N2714" s="42"/>
-      <c r="V2714" s="42"/>
-    </row>
-    <row r="2715" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2715" s="45"/>
-      <c r="N2715" s="42"/>
-      <c r="V2715" s="42"/>
-    </row>
-    <row r="2716" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2716" s="45"/>
-      <c r="N2716" s="42"/>
-      <c r="V2716" s="42"/>
-    </row>
-    <row r="2717" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2717" s="45"/>
-      <c r="N2717" s="42"/>
-      <c r="V2717" s="42"/>
-    </row>
-    <row r="2718" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2718" s="45"/>
-      <c r="N2718" s="42"/>
-      <c r="V2718" s="42"/>
-    </row>
-    <row r="2719" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2719" s="45"/>
-      <c r="N2719" s="42"/>
-      <c r="V2719" s="42"/>
-    </row>
-    <row r="2720" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2720" s="45"/>
-      <c r="N2720" s="42"/>
-      <c r="V2720" s="42"/>
-    </row>
-    <row r="2721" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2721" s="45"/>
-      <c r="N2721" s="42"/>
-      <c r="V2721" s="42"/>
-    </row>
-    <row r="2722" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2722" s="45"/>
-      <c r="N2722" s="42"/>
-      <c r="V2722" s="42"/>
-    </row>
-    <row r="2723" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2723" s="45"/>
-      <c r="N2723" s="42"/>
-      <c r="V2723" s="42"/>
-    </row>
-    <row r="2724" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2724" s="45"/>
-      <c r="N2724" s="42"/>
-      <c r="V2724" s="42"/>
-    </row>
-    <row r="2725" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2725" s="45"/>
-      <c r="N2725" s="42"/>
-      <c r="V2725" s="42"/>
-    </row>
-    <row r="2726" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2726" s="45"/>
-      <c r="N2726" s="42"/>
-      <c r="V2726" s="42"/>
-    </row>
-    <row r="2727" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2727" s="45"/>
-      <c r="N2727" s="42"/>
-      <c r="V2727" s="42"/>
-    </row>
-    <row r="2728" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2728" s="45"/>
-      <c r="N2728" s="42"/>
-      <c r="V2728" s="42"/>
     </row>
   </sheetData>
   <autoFilter ref="C1:V2126" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
nmv 09 11 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 6.6 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 6.6 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F2F074-1BF1-49BC-8582-238A643A4ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AA756D-4C95-4C59-9B6E-07D1F7366459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5488" uniqueCount="1320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5491" uniqueCount="1323">
   <si>
     <t>Passage</t>
   </si>
@@ -4000,6 +4000,15 @@
       </rPr>
       <t>aBi cCandaH??</t>
     </r>
+  </si>
+  <si>
+    <t>patha rtasya</t>
+  </si>
+  <si>
+    <t>viT, vil laBate</t>
+  </si>
+  <si>
+    <t>kampam as per samhita</t>
   </si>
 </sst>
 </file>
@@ -4170,7 +4179,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4219,6 +4228,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -4247,7 +4268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4439,23 +4460,14 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4739,10 +4751,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2080" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="T2127" sqref="T2127"/>
+      <selection pane="bottomLeft" activeCell="Q2133" sqref="Q2133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -9898,7 +9910,7 @@
         <f t="shared" si="5"/>
         <v>119</v>
       </c>
-      <c r="N120" s="42" t="s">
+      <c r="N120" s="65" t="s">
         <v>205</v>
       </c>
       <c r="O120" s="7"/>
@@ -9911,7 +9923,9 @@
       <c r="V120" s="42"/>
     </row>
     <row r="121" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A121" s="8"/>
+      <c r="A121" s="8" t="s">
+        <v>1320</v>
+      </c>
       <c r="D121" s="22"/>
       <c r="H121" s="49" t="s">
         <v>71</v>
@@ -9934,7 +9948,7 @@
         <f t="shared" si="5"/>
         <v>120</v>
       </c>
-      <c r="N121" s="42" t="s">
+      <c r="N121" s="65" t="s">
         <v>202</v>
       </c>
       <c r="O121" s="8"/>
@@ -31219,34 +31233,34 @@
       </c>
     </row>
     <row r="743" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I743" s="65" t="s">
+      <c r="I743" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="J743" s="66">
+      <c r="J743" s="48">
         <v>16</v>
       </c>
-      <c r="K743" s="67">
+      <c r="K743" s="6">
         <f t="shared" si="33"/>
         <v>742</v>
       </c>
-      <c r="L743" s="67">
+      <c r="L743" s="6">
         <v>1</v>
       </c>
-      <c r="M743" s="67">
+      <c r="M743" s="6">
         <f t="shared" si="35"/>
         <v>101</v>
       </c>
-      <c r="N743" s="68" t="s">
+      <c r="N743" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="O743" s="69"/>
-      <c r="P743" s="70"/>
-      <c r="Q743" s="70"/>
-      <c r="R743" s="70"/>
-      <c r="S743" s="70"/>
-      <c r="T743" s="70"/>
-      <c r="U743" s="70"/>
-      <c r="V743" s="68"/>
+      <c r="O743" s="7"/>
+      <c r="P743" s="8"/>
+      <c r="Q743" s="8"/>
+      <c r="R743" s="8"/>
+      <c r="S743" s="8"/>
+      <c r="T743" s="8"/>
+      <c r="U743" s="8"/>
+      <c r="V743" s="42"/>
     </row>
     <row r="744" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I744" s="45" t="s">
@@ -40922,7 +40936,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="1041" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1041" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="H1041" s="32"/>
       <c r="I1041" s="45" t="s">
         <v>41</v>
@@ -40954,7 +40968,7 @@
       <c r="U1041" s="8"/>
       <c r="V1041" s="42"/>
     </row>
-    <row r="1042" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1042" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="G1042" s="50" t="s">
         <v>117</v>
       </c>
@@ -40990,7 +41004,7 @@
       <c r="U1042" s="8"/>
       <c r="V1042" s="42"/>
     </row>
-    <row r="1043" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1043" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1043" s="50" t="s">
         <v>114</v>
       </c>
@@ -41021,7 +41035,7 @@
         <f t="shared" si="50"/>
         <v>121</v>
       </c>
-      <c r="N1043" s="42" t="s">
+      <c r="N1043" s="65" t="s">
         <v>630</v>
       </c>
       <c r="O1043" s="7"/>
@@ -41033,7 +41047,10 @@
       <c r="U1043" s="8"/>
       <c r="V1043" s="42"/>
     </row>
-    <row r="1044" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1044" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A1044" s="8" t="s">
+        <v>1321</v>
+      </c>
       <c r="E1044" s="50" t="s">
         <v>114</v>
       </c>
@@ -41064,7 +41081,7 @@
         <f t="shared" si="50"/>
         <v>122</v>
       </c>
-      <c r="N1044" s="42" t="s">
+      <c r="N1044" s="65" t="s">
         <v>636</v>
       </c>
       <c r="O1044" s="7"/>
@@ -41076,7 +41093,7 @@
       <c r="U1044" s="8"/>
       <c r="V1044" s="42"/>
     </row>
-    <row r="1045" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1045" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="H1045" s="49" t="s">
         <v>96</v>
       </c>
@@ -41110,7 +41127,7 @@
       <c r="U1045" s="8"/>
       <c r="V1045" s="42"/>
     </row>
-    <row r="1046" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1046" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1046" s="45" t="s">
         <v>41</v>
       </c>
@@ -41141,7 +41158,7 @@
       <c r="U1046" s="8"/>
       <c r="V1046" s="42"/>
     </row>
-    <row r="1047" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1047" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1047" s="45" t="s">
         <v>41</v>
       </c>
@@ -41172,7 +41189,7 @@
       <c r="U1047" s="8"/>
       <c r="V1047" s="42"/>
     </row>
-    <row r="1048" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1048" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1048" s="45" t="s">
         <v>41</v>
       </c>
@@ -41203,7 +41220,7 @@
       <c r="U1048" s="8"/>
       <c r="V1048" s="42"/>
     </row>
-    <row r="1049" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1049" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1049" s="45" t="s">
         <v>41</v>
       </c>
@@ -41234,7 +41251,7 @@
       <c r="U1049" s="8"/>
       <c r="V1049" s="42"/>
     </row>
-    <row r="1050" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1050" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1050" s="45" t="s">
         <v>41</v>
       </c>
@@ -41267,7 +41284,7 @@
       <c r="U1050" s="8"/>
       <c r="V1050" s="42"/>
     </row>
-    <row r="1051" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1051" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1051" s="45" t="s">
         <v>41</v>
       </c>
@@ -41298,7 +41315,7 @@
       <c r="U1051" s="8"/>
       <c r="V1051" s="42"/>
     </row>
-    <row r="1052" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1052" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1052" s="45" t="s">
         <v>41</v>
       </c>
@@ -41329,7 +41346,7 @@
       <c r="U1052" s="8"/>
       <c r="V1052" s="42"/>
     </row>
-    <row r="1053" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1053" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1053" s="45" t="s">
         <v>41</v>
       </c>
@@ -41360,7 +41377,7 @@
       <c r="U1053" s="8"/>
       <c r="V1053" s="42"/>
     </row>
-    <row r="1054" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1054" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1054" s="45" t="s">
         <v>41</v>
       </c>
@@ -41391,7 +41408,7 @@
       <c r="U1054" s="8"/>
       <c r="V1054" s="42"/>
     </row>
-    <row r="1055" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1055" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1055" s="45" t="s">
         <v>41</v>
       </c>
@@ -41426,7 +41443,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="1056" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1056" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1056" s="45" t="s">
         <v>41</v>
       </c>
@@ -52405,7 +52422,7 @@
       <c r="U1392" s="8"/>
       <c r="V1392" s="42"/>
     </row>
-    <row r="1393" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1393" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1393" s="37"/>
       <c r="I1393" s="45" t="s">
         <v>48</v>
@@ -52441,7 +52458,7 @@
       <c r="U1393" s="8"/>
       <c r="V1393" s="42"/>
     </row>
-    <row r="1394" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1394" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1394" s="37"/>
       <c r="I1394" s="45" t="s">
         <v>48</v>
@@ -52475,7 +52492,7 @@
       <c r="U1394" s="8"/>
       <c r="V1394" s="42"/>
     </row>
-    <row r="1395" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1395" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1395" s="37"/>
       <c r="I1395" s="45" t="s">
         <v>48</v>
@@ -52507,7 +52524,7 @@
       <c r="U1395" s="8"/>
       <c r="V1395" s="42"/>
     </row>
-    <row r="1396" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1396" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1396" s="37"/>
       <c r="I1396" s="45" t="s">
         <v>48</v>
@@ -52543,7 +52560,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="1397" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1397" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1397" s="37"/>
       <c r="I1397" s="45" t="s">
         <v>48</v>
@@ -52579,7 +52596,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="1398" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1398" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1398" s="37"/>
       <c r="I1398" s="45" t="s">
         <v>48</v>
@@ -52615,7 +52632,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="1399" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1399" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1399" s="37"/>
       <c r="I1399" s="45" t="s">
         <v>48</v>
@@ -52647,7 +52664,7 @@
       <c r="U1399" s="8"/>
       <c r="V1399" s="42"/>
     </row>
-    <row r="1400" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1400" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1400" s="37"/>
       <c r="I1400" s="45" t="s">
         <v>48</v>
@@ -52679,7 +52696,7 @@
       <c r="U1400" s="8"/>
       <c r="V1400" s="42"/>
     </row>
-    <row r="1401" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1401" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1401" s="37"/>
       <c r="I1401" s="45" t="s">
         <v>48</v>
@@ -52715,7 +52732,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="1402" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1402" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1402" s="37"/>
       <c r="H1402" s="32"/>
       <c r="I1402" s="45" t="s">
@@ -52746,7 +52763,7 @@
       <c r="U1402" s="8"/>
       <c r="V1402" s="42"/>
     </row>
-    <row r="1403" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1403" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1403" s="37"/>
       <c r="H1403" s="32"/>
       <c r="I1403" s="45" t="s">
@@ -52779,7 +52796,7 @@
       <c r="U1403" s="8"/>
       <c r="V1403" s="42"/>
     </row>
-    <row r="1404" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1404" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1404" s="37"/>
       <c r="H1404" s="32"/>
       <c r="I1404" s="45" t="s">
@@ -52812,7 +52829,10 @@
       <c r="U1404" s="8"/>
       <c r="V1404" s="42"/>
     </row>
-    <row r="1405" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1405" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A1405" s="8" t="s">
+        <v>1322</v>
+      </c>
       <c r="C1405" s="37"/>
       <c r="F1405" s="50" t="s">
         <v>131</v>
@@ -52836,7 +52856,7 @@
         <f t="shared" si="65"/>
         <v>4</v>
       </c>
-      <c r="N1405" s="43" t="s">
+      <c r="N1405" s="66" t="s">
         <v>303</v>
       </c>
       <c r="O1405" s="7"/>
@@ -52848,7 +52868,7 @@
       <c r="U1405" s="8"/>
       <c r="V1405" s="42"/>
     </row>
-    <row r="1406" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1406" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1406" s="37"/>
       <c r="F1406" s="50" t="s">
         <v>131</v>
@@ -52872,7 +52892,7 @@
         <f t="shared" si="65"/>
         <v>5</v>
       </c>
-      <c r="N1406" s="42" t="s">
+      <c r="N1406" s="67" t="s">
         <v>185</v>
       </c>
       <c r="O1406" s="7" t="s">
@@ -52886,7 +52906,7 @@
       <c r="U1406" s="8"/>
       <c r="V1406" s="42"/>
     </row>
-    <row r="1407" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1407" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1407" s="37"/>
       <c r="F1407" s="50" t="s">
         <v>131</v>
@@ -52910,7 +52930,7 @@
         <f t="shared" si="65"/>
         <v>6</v>
       </c>
-      <c r="N1407" s="42" t="s">
+      <c r="N1407" s="67" t="s">
         <v>788</v>
       </c>
       <c r="O1407" s="7"/>
@@ -52922,7 +52942,7 @@
       <c r="U1407" s="8"/>
       <c r="V1407" s="42"/>
     </row>
-    <row r="1408" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1408" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1408" s="37"/>
       <c r="F1408" s="50" t="s">
         <v>131</v>

</xml_diff>

<commit_message>
nmv 24 01 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 6.6 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 6.6 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97559533-2463-42A5-A28C-110875A01F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43133A3A-7302-466C-94AB-08B6A606443A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5491" uniqueCount="1322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5491" uniqueCount="1323">
   <si>
     <t>Passage</t>
   </si>
@@ -4006,6 +4006,9 @@
   </si>
   <si>
     <t>uqdgAqtRuBya#H</t>
+  </si>
+  <si>
+    <t>praqjApa#tim</t>
   </si>
 </sst>
 </file>
@@ -4748,10 +4751,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1369" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1905" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="T2129" sqref="T2129"/>
+      <selection pane="bottomLeft" activeCell="N1908" sqref="N1908"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -66855,8 +66858,8 @@
         <f t="shared" si="89"/>
         <v>79</v>
       </c>
-      <c r="N1908" s="42" t="s">
-        <v>295</v>
+      <c r="N1908" s="43" t="s">
+        <v>1322</v>
       </c>
       <c r="O1908" s="8" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
nmv 26 01 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 6.6 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 6.6 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43133A3A-7302-466C-94AB-08B6A606443A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8C6F16-8A5D-421F-9EE8-64C286EC5349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4752,9 +4752,9 @@
   <dimension ref="A1:V2126"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1905" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1908" sqref="N1908"/>
+      <selection pane="bottomLeft" activeCell="N112" sqref="N112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -9609,8 +9609,8 @@
         <f t="shared" si="5"/>
         <v>111</v>
       </c>
-      <c r="N112" s="58" t="s">
-        <v>151</v>
+      <c r="N112" s="60" t="s">
+        <v>180</v>
       </c>
       <c r="O112" s="8"/>
       <c r="P112" s="7"/>

</xml_diff>

<commit_message>
nmv 02 02 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 6.6 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 6.6 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2EE87C-77ED-42D3-96BE-E201645E3E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D8D87A-2890-4BA1-B4DC-99C5FC9355B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5491" uniqueCount="1322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5491" uniqueCount="1323">
   <si>
     <t>Passage</t>
   </si>
@@ -3427,9 +3427,6 @@
   </si>
   <si>
     <t>Aqkrama#NaqmityA$ - krama#Nam</t>
-  </si>
-  <si>
-    <t>sama#ShTyaq itiq saM - aqShTyaiq</t>
   </si>
   <si>
     <t xml:space="preserve">dve itiq dve </t>
@@ -4006,6 +4003,12 @@
   </si>
   <si>
     <t>apa#bar.hiShAqvityapa# - baqrq.hiqShauq</t>
+  </si>
+  <si>
+    <t>sama#ShTyai</t>
+  </si>
+  <si>
+    <t>sama#ShTyAq itiq saM - aqShTyaiq</t>
   </si>
 </sst>
 </file>
@@ -4749,9 +4752,9 @@
   <dimension ref="A1:V2126"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A510" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A735" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V510" sqref="V510"/>
+      <selection pane="bottomLeft" activeCell="V746" sqref="V746"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -6816,7 +6819,7 @@
         <v>38</v>
       </c>
       <c r="N39" s="43" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="O39" s="8" t="s">
         <v>64</v>
@@ -7187,7 +7190,7 @@
         <v>85</v>
       </c>
       <c r="T48" s="15" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="U48" s="15"/>
       <c r="V48" s="42"/>
@@ -8140,7 +8143,7 @@
     </row>
     <row r="73" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="C73" s="10"/>
       <c r="D73" s="21"/>
@@ -9141,7 +9144,7 @@
       <c r="S100" s="8"/>
       <c r="T100" s="8"/>
       <c r="U100" s="8" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="V100" s="42"/>
     </row>
@@ -9921,7 +9924,7 @@
     </row>
     <row r="121" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A121" s="8" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="D121" s="22"/>
       <c r="H121" s="49" t="s">
@@ -11508,7 +11511,7 @@
         <v>85</v>
       </c>
       <c r="T167" s="8" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="U167" s="8"/>
       <c r="V167" s="42"/>
@@ -13979,7 +13982,7 @@
         <v>238</v>
       </c>
       <c r="N239" s="42" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="O239" s="7"/>
       <c r="P239" s="8" t="s">
@@ -13991,7 +13994,7 @@
       <c r="T239" s="8"/>
       <c r="U239" s="8"/>
       <c r="V239" s="42" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="240" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -17526,7 +17529,7 @@
     </row>
     <row r="343" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A343" s="60" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="D343" s="22"/>
       <c r="F343" s="50" t="s">
@@ -17554,7 +17557,7 @@
         <v>104</v>
       </c>
       <c r="N343" s="60" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="O343" s="8" t="s">
         <v>64</v>
@@ -18805,10 +18808,10 @@
       <c r="Q378" s="8"/>
       <c r="R378" s="8"/>
       <c r="S378" s="8" t="s">
+        <v>1297</v>
+      </c>
+      <c r="T378" s="8" t="s">
         <v>1298</v>
-      </c>
-      <c r="T378" s="8" t="s">
-        <v>1299</v>
       </c>
       <c r="U378" s="8"/>
       <c r="V378" s="42"/>
@@ -19951,7 +19954,7 @@
         <v>31</v>
       </c>
       <c r="N411" s="43" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="O411" s="7"/>
       <c r="P411" s="8"/>
@@ -22789,7 +22792,7 @@
       <c r="T493" s="8"/>
       <c r="U493" s="8"/>
       <c r="V493" s="43" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="494" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22857,7 +22860,7 @@
         <v>85</v>
       </c>
       <c r="T495" s="8" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="U495" s="8"/>
       <c r="V495" s="42"/>
@@ -23374,7 +23377,7 @@
       <c r="T510" s="8"/>
       <c r="U510" s="8"/>
       <c r="V510" s="43" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="511" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24705,7 +24708,7 @@
         <v>85</v>
       </c>
       <c r="T548" s="8" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="U548" s="8"/>
       <c r="V548" s="42"/>
@@ -24880,7 +24883,7 @@
         <v>85</v>
       </c>
       <c r="T553" s="8" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="U553" s="8"/>
       <c r="V553" s="42"/>
@@ -26985,7 +26988,7 @@
         <v>111</v>
       </c>
       <c r="T615" s="8" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="U615" s="8"/>
       <c r="V615" s="42"/>
@@ -27922,7 +27925,7 @@
       <c r="T642" s="8"/>
       <c r="U642" s="8"/>
       <c r="V642" s="42" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="643" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -29138,7 +29141,7 @@
         <v>36</v>
       </c>
       <c r="N678" s="43" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="O678" s="8" t="s">
         <v>64</v>
@@ -31213,8 +31216,8 @@
         <f t="shared" si="35"/>
         <v>100</v>
       </c>
-      <c r="N742" s="42" t="s">
-        <v>266</v>
+      <c r="N742" s="43" t="s">
+        <v>1321</v>
       </c>
       <c r="O742" s="8" t="s">
         <v>64</v>
@@ -31225,8 +31228,8 @@
       <c r="S742" s="8"/>
       <c r="T742" s="8"/>
       <c r="U742" s="8"/>
-      <c r="V742" s="42" t="s">
-        <v>1133</v>
+      <c r="V742" s="43" t="s">
+        <v>1322</v>
       </c>
     </row>
     <row r="743" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31353,7 +31356,7 @@
       <c r="T746" s="8"/>
       <c r="U746" s="8"/>
       <c r="V746" s="42" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="747" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31388,7 +31391,7 @@
       <c r="T747" s="8"/>
       <c r="U747" s="8"/>
       <c r="V747" s="42" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="748" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31423,7 +31426,7 @@
       <c r="T748" s="8"/>
       <c r="U748" s="8"/>
       <c r="V748" s="42" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="749" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31520,7 +31523,7 @@
       <c r="T751" s="8"/>
       <c r="U751" s="8"/>
       <c r="V751" s="42" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="752" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31555,7 +31558,7 @@
       <c r="T752" s="8"/>
       <c r="U752" s="8"/>
       <c r="V752" s="42" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="753" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31809,7 +31812,7 @@
       <c r="T760" s="8"/>
       <c r="U760" s="8"/>
       <c r="V760" s="42" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="761" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31972,7 +31975,7 @@
       <c r="T765" s="8"/>
       <c r="U765" s="8"/>
       <c r="V765" s="42" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="766" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32226,7 +32229,7 @@
       <c r="T773" s="8"/>
       <c r="U773" s="8"/>
       <c r="V773" s="42" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="774" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32646,7 +32649,7 @@
       <c r="T786" s="8"/>
       <c r="U786" s="8"/>
       <c r="V786" s="42" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="787" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33174,7 +33177,7 @@
       <c r="T802" s="8"/>
       <c r="U802" s="8"/>
       <c r="V802" s="42" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="803" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33350,7 +33353,7 @@
       <c r="T807" s="8"/>
       <c r="U807" s="8"/>
       <c r="V807" s="42" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="808" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33388,7 +33391,7 @@
       <c r="T808" s="8"/>
       <c r="U808" s="8"/>
       <c r="V808" s="42" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="809" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33500,7 +33503,7 @@
       <c r="T811" s="8"/>
       <c r="U811" s="8"/>
       <c r="V811" s="42" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="812" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33544,7 +33547,7 @@
       <c r="T812" s="8"/>
       <c r="U812" s="8"/>
       <c r="V812" s="42" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="813" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33588,7 +33591,7 @@
       <c r="T813" s="8"/>
       <c r="U813" s="8"/>
       <c r="V813" s="42" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="814" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33750,7 +33753,7 @@
       <c r="T818" s="8"/>
       <c r="U818" s="8"/>
       <c r="V818" s="42" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="819" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33822,7 +33825,7 @@
       <c r="T820" s="8"/>
       <c r="U820" s="8"/>
       <c r="V820" s="42" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="821" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34083,7 +34086,7 @@
       <c r="T828" s="8"/>
       <c r="U828" s="8"/>
       <c r="V828" s="42" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="829" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34368,7 +34371,7 @@
         <v>111</v>
       </c>
       <c r="T837" s="8" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="U837" s="8"/>
       <c r="V837" s="42"/>
@@ -35205,7 +35208,7 @@
       <c r="T863" s="8"/>
       <c r="U863" s="8"/>
       <c r="V863" s="42" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="864" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35337,7 +35340,7 @@
       <c r="T867" s="8"/>
       <c r="U867" s="8"/>
       <c r="V867" s="42" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="868" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35660,7 +35663,7 @@
       <c r="T877" s="8"/>
       <c r="U877" s="8"/>
       <c r="V877" s="42" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="878" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35886,7 +35889,7 @@
       <c r="T884" s="8"/>
       <c r="U884" s="8"/>
       <c r="V884" s="42" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="885" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35921,7 +35924,7 @@
       <c r="T885" s="8"/>
       <c r="U885" s="8"/>
       <c r="V885" s="42" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="886" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35987,7 +35990,7 @@
       <c r="T887" s="8"/>
       <c r="U887" s="8"/>
       <c r="V887" s="42" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="888" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36022,7 +36025,7 @@
       <c r="T888" s="8"/>
       <c r="U888" s="8"/>
       <c r="V888" s="42" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="889" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36088,7 +36091,7 @@
       <c r="T890" s="8"/>
       <c r="U890" s="8"/>
       <c r="V890" s="42" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="891" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36894,7 +36897,7 @@
       <c r="T915" s="8"/>
       <c r="U915" s="8"/>
       <c r="V915" s="42" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="916" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36960,7 +36963,7 @@
       <c r="T917" s="8"/>
       <c r="U917" s="8"/>
       <c r="V917" s="42" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="918" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37090,7 +37093,7 @@
       <c r="T921" s="8"/>
       <c r="U921" s="8"/>
       <c r="V921" s="42" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="922" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37113,7 +37116,7 @@
         <v>280</v>
       </c>
       <c r="N922" s="42" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O922" s="8" t="s">
         <v>64</v>
@@ -37127,7 +37130,7 @@
       <c r="T922" s="8"/>
       <c r="U922" s="8"/>
       <c r="V922" s="42" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="923" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37160,7 +37163,7 @@
       <c r="T923" s="8"/>
       <c r="U923" s="8"/>
       <c r="V923" s="42" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="924" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39284,7 +39287,7 @@
       <c r="T990" s="8"/>
       <c r="U990" s="8"/>
       <c r="V990" s="42" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="991" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39350,7 +39353,7 @@
       <c r="T992" s="8"/>
       <c r="U992" s="8"/>
       <c r="V992" s="42" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="993" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39919,7 +39922,7 @@
       <c r="T1009" s="8"/>
       <c r="U1009" s="8"/>
       <c r="V1009" s="42" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="1010" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39955,7 +39958,7 @@
       <c r="T1010" s="8"/>
       <c r="U1010" s="8"/>
       <c r="V1010" s="42" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="1011" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40029,7 +40032,7 @@
       <c r="T1012" s="8"/>
       <c r="U1012" s="8"/>
       <c r="V1012" s="42" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="1013" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40448,7 +40451,7 @@
       <c r="T1025" s="8"/>
       <c r="U1025" s="8"/>
       <c r="V1025" s="42" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="1026" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40547,7 +40550,7 @@
       <c r="T1028" s="8"/>
       <c r="U1028" s="8"/>
       <c r="V1028" s="42" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="1029" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40930,7 +40933,7 @@
       <c r="T1040" s="8"/>
       <c r="U1040" s="8"/>
       <c r="V1040" s="42" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="1041" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41046,7 +41049,7 @@
     </row>
     <row r="1044" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1044" s="8" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="E1044" s="50" t="s">
         <v>114</v>
@@ -41437,7 +41440,7 @@
       <c r="T1055" s="8"/>
       <c r="U1055" s="8"/>
       <c r="V1055" s="42" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="1056" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41598,7 +41601,7 @@
       <c r="T1060" s="8"/>
       <c r="U1060" s="8"/>
       <c r="V1060" s="42" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="1061" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42070,7 +42073,7 @@
       <c r="T1075" s="8"/>
       <c r="U1075" s="8"/>
       <c r="V1075" s="42" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="1076" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42232,7 +42235,7 @@
       <c r="T1080" s="8"/>
       <c r="U1080" s="8"/>
       <c r="V1080" s="42" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="1081" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42726,7 +42729,7 @@
       <c r="T1095" s="8"/>
       <c r="U1095" s="8"/>
       <c r="V1095" s="42" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="1096" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42825,7 +42828,7 @@
       <c r="T1098" s="8"/>
       <c r="U1098" s="8"/>
       <c r="V1098" s="42" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="1099" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43091,7 +43094,7 @@
       <c r="T1106" s="8"/>
       <c r="U1106" s="8"/>
       <c r="V1106" s="42" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="1107" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43158,7 +43161,7 @@
       <c r="T1108" s="8"/>
       <c r="U1108" s="8"/>
       <c r="V1108" s="42" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="1109" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43181,7 +43184,7 @@
         <v>187</v>
       </c>
       <c r="N1109" s="42" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="O1109" s="8" t="s">
         <v>64</v>
@@ -43195,7 +43198,7 @@
       <c r="T1109" s="8"/>
       <c r="U1109" s="8"/>
       <c r="V1109" s="42" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="1110" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43383,7 +43386,7 @@
       <c r="T1115" s="8"/>
       <c r="U1115" s="8"/>
       <c r="V1115" s="42" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="1116" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43609,7 +43612,7 @@
       <c r="T1122" s="8"/>
       <c r="U1122" s="8"/>
       <c r="V1122" s="42" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="1123" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43644,7 +43647,7 @@
       <c r="T1123" s="8"/>
       <c r="U1123" s="8"/>
       <c r="V1123" s="42" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="1124" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43679,7 +43682,7 @@
       <c r="T1124" s="8"/>
       <c r="U1124" s="8"/>
       <c r="V1124" s="42" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="1125" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44059,7 +44062,7 @@
       <c r="T1136" s="8"/>
       <c r="U1136" s="8"/>
       <c r="V1136" s="42" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="1137" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44221,12 +44224,12 @@
       <c r="T1141" s="8"/>
       <c r="U1141" s="8"/>
       <c r="V1141" s="42" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="1142" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1142" s="8" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="I1142" s="45" t="s">
         <v>43</v>
@@ -44450,7 +44453,7 @@
       <c r="T1148" s="8"/>
       <c r="U1148" s="8"/>
       <c r="V1148" s="42" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="1149" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44486,7 +44489,7 @@
       <c r="T1149" s="8"/>
       <c r="U1149" s="8"/>
       <c r="V1149" s="42" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="1150" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44623,7 +44626,7 @@
       <c r="T1153" s="8"/>
       <c r="U1153" s="8"/>
       <c r="V1153" s="42" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="1154" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44977,7 +44980,7 @@
       <c r="T1164" s="8"/>
       <c r="U1164" s="8"/>
       <c r="V1164" s="42" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="1165" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45958,7 +45961,7 @@
       <c r="T1195" s="8"/>
       <c r="U1195" s="8"/>
       <c r="V1195" s="42" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="1196" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46146,7 +46149,7 @@
       <c r="T1201" s="8"/>
       <c r="U1201" s="8"/>
       <c r="V1201" s="42" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="1202" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46309,7 +46312,7 @@
     </row>
     <row r="1207" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1207" s="62" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="B1207" s="63"/>
       <c r="C1207" s="51"/>
@@ -46349,7 +46352,7 @@
       <c r="T1207" s="8"/>
       <c r="U1207" s="8"/>
       <c r="V1207" s="42" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="1208" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46542,7 +46545,7 @@
       <c r="T1213" s="8"/>
       <c r="U1213" s="8"/>
       <c r="V1213" s="42" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1214" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46720,7 +46723,7 @@
         <v>24</v>
       </c>
       <c r="N1219" s="43" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="O1219" s="8" t="s">
         <v>64</v>
@@ -46732,7 +46735,7 @@
       <c r="T1219" s="8"/>
       <c r="U1219" s="8"/>
       <c r="V1219" s="42" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="1220" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46798,7 +46801,7 @@
       <c r="T1221" s="8"/>
       <c r="U1221" s="8"/>
       <c r="V1221" s="42" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="1222" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47116,7 +47119,7 @@
       <c r="T1231" s="8"/>
       <c r="U1231" s="8"/>
       <c r="V1231" s="42" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="1232" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47140,7 +47143,7 @@
         <v>37</v>
       </c>
       <c r="N1232" s="43" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="O1232" s="8" t="s">
         <v>64</v>
@@ -47152,7 +47155,7 @@
       <c r="T1232" s="8"/>
       <c r="U1232" s="8"/>
       <c r="V1232" s="42" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="1233" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47218,7 +47221,7 @@
       <c r="T1234" s="8"/>
       <c r="U1234" s="8"/>
       <c r="V1234" s="42" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="1235" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47408,7 +47411,7 @@
       <c r="T1240" s="8"/>
       <c r="U1240" s="8"/>
       <c r="V1240" s="42" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="1241" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47909,7 +47912,7 @@
       <c r="T1256" s="8"/>
       <c r="U1256" s="8"/>
       <c r="V1256" s="42" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="1257" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47944,7 +47947,7 @@
       <c r="T1257" s="8"/>
       <c r="U1257" s="8"/>
       <c r="V1257" s="42" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="1258" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48010,7 +48013,7 @@
       <c r="T1259" s="8"/>
       <c r="U1259" s="8"/>
       <c r="V1259" s="42" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="1260" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48237,7 +48240,7 @@
       <c r="T1266" s="8"/>
       <c r="U1266" s="8"/>
       <c r="V1266" s="42" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="1267" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48436,7 +48439,7 @@
       <c r="T1272" s="8"/>
       <c r="U1272" s="8"/>
       <c r="V1272" s="42" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="1273" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48690,7 +48693,7 @@
       <c r="T1280" s="8"/>
       <c r="U1280" s="8"/>
       <c r="V1280" s="42" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="1281" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48806,7 +48809,7 @@
         <v>89</v>
       </c>
       <c r="N1284" s="42" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="O1284" s="8" t="s">
         <v>64</v>
@@ -48819,10 +48822,10 @@
       <c r="S1284" s="8"/>
       <c r="T1284" s="8"/>
       <c r="U1284" s="8" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="V1284" s="42" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="1285" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49228,7 +49231,7 @@
       <c r="T1297" s="8"/>
       <c r="U1297" s="8"/>
       <c r="V1297" s="42" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="1298" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49358,7 +49361,7 @@
       <c r="T1301" s="8"/>
       <c r="U1301" s="8"/>
       <c r="V1301" s="42" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="1302" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49562,7 +49565,7 @@
       <c r="T1307" s="8"/>
       <c r="U1307" s="8"/>
       <c r="V1307" s="42" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="1308" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50054,7 +50057,7 @@
       <c r="T1322" s="8"/>
       <c r="U1322" s="8"/>
       <c r="V1322" s="42" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="1323" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50122,7 +50125,7 @@
       <c r="T1324" s="8"/>
       <c r="U1324" s="8"/>
       <c r="V1324" s="42" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="1325" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50159,7 +50162,7 @@
       <c r="T1325" s="8"/>
       <c r="U1325" s="8"/>
       <c r="V1325" s="42" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="1326" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50295,7 +50298,7 @@
       <c r="T1329" s="8"/>
       <c r="U1329" s="8"/>
       <c r="V1329" s="42" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="1330" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50399,7 +50402,7 @@
       <c r="S1332" s="8"/>
       <c r="T1332" s="8"/>
       <c r="V1332" s="42" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="1333" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50429,7 +50432,7 @@
         <v>138</v>
       </c>
       <c r="N1333" s="53" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="O1333" s="7"/>
       <c r="P1333" s="8"/>
@@ -50538,7 +50541,7 @@
         <v>141</v>
       </c>
       <c r="N1336" s="53" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="O1336" s="8"/>
       <c r="P1336" s="8"/>
@@ -50716,7 +50719,7 @@
       <c r="T1341" s="8"/>
       <c r="U1341" s="8"/>
       <c r="V1341" s="42" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="1342" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50784,7 +50787,7 @@
       <c r="T1343" s="8"/>
       <c r="U1343" s="8"/>
       <c r="V1343" s="42" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="1344" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50915,7 +50918,7 @@
       <c r="T1347" s="8"/>
       <c r="U1347" s="8"/>
       <c r="V1347" s="42" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="1348" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51015,7 +51018,7 @@
       <c r="T1350" s="8"/>
       <c r="U1350" s="8"/>
       <c r="V1350" s="42" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="1351" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51344,7 +51347,7 @@
       <c r="T1360" s="8"/>
       <c r="U1360" s="8"/>
       <c r="V1360" s="42" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="1361" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51414,7 +51417,7 @@
       <c r="T1362" s="8"/>
       <c r="U1362" s="8"/>
       <c r="V1362" s="42" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="1363" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51580,7 +51583,7 @@
       <c r="T1367" s="8"/>
       <c r="U1367" s="8"/>
       <c r="V1367" s="42" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="1368" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51651,7 +51654,7 @@
       <c r="T1369" s="8"/>
       <c r="U1369" s="8"/>
       <c r="V1369" s="43" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="1370" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51754,7 +51757,7 @@
       <c r="T1372" s="8"/>
       <c r="U1372" s="8"/>
       <c r="V1372" s="42" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="1373" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51823,7 +51826,7 @@
       <c r="T1374" s="8"/>
       <c r="U1374" s="8"/>
       <c r="V1374" s="42" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="1375" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51891,7 +51894,7 @@
       <c r="T1376" s="8"/>
       <c r="U1376" s="8"/>
       <c r="V1376" s="42" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="1377" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52284,7 +52287,7 @@
       <c r="T1388" s="8"/>
       <c r="U1388" s="8"/>
       <c r="V1388" s="42" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="1389" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52352,7 +52355,7 @@
       <c r="T1390" s="8"/>
       <c r="U1390" s="8"/>
       <c r="V1390" s="42" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="1391" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52450,7 +52453,7 @@
         <v>85</v>
       </c>
       <c r="T1393" s="8" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="U1393" s="8"/>
       <c r="V1393" s="42"/>
@@ -52554,7 +52557,7 @@
       <c r="T1396" s="8"/>
       <c r="U1396" s="8"/>
       <c r="V1396" s="42" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="1397" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52626,7 +52629,7 @@
       <c r="T1398" s="8"/>
       <c r="U1398" s="8"/>
       <c r="V1398" s="42" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="1399" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52726,7 +52729,7 @@
       <c r="T1401" s="8"/>
       <c r="U1401" s="8"/>
       <c r="V1401" s="42" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1402" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52828,7 +52831,7 @@
     </row>
     <row r="1405" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1405" s="8" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="C1405" s="37"/>
       <c r="F1405" s="50" t="s">
@@ -53039,7 +53042,7 @@
       <c r="T1410" s="8"/>
       <c r="U1410" s="8"/>
       <c r="V1410" s="42" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="1411" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53107,7 +53110,7 @@
       <c r="T1412" s="8"/>
       <c r="U1412" s="8"/>
       <c r="V1412" s="42" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="1413" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53207,7 +53210,7 @@
       <c r="T1415" s="8"/>
       <c r="U1415" s="8"/>
       <c r="V1415" s="42" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="1416" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53243,7 +53246,7 @@
       <c r="T1416" s="8"/>
       <c r="U1416" s="8"/>
       <c r="V1416" s="42" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="1417" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53311,7 +53314,7 @@
       <c r="T1418" s="8"/>
       <c r="U1418" s="8"/>
       <c r="V1418" s="42" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="1419" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53731,7 +53734,7 @@
       <c r="T1431" s="8"/>
       <c r="U1431" s="8"/>
       <c r="V1431" s="42" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="1432" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53799,7 +53802,7 @@
       <c r="T1433" s="8"/>
       <c r="U1433" s="8"/>
       <c r="V1433" s="42" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="1434" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53963,7 +53966,7 @@
       <c r="T1438" s="8"/>
       <c r="U1438" s="8"/>
       <c r="V1438" s="42" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="1439" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53999,7 +54002,7 @@
       <c r="T1439" s="8"/>
       <c r="U1439" s="8"/>
       <c r="V1439" s="42" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="1440" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54516,7 +54519,7 @@
       <c r="T1455" s="8"/>
       <c r="U1455" s="8"/>
       <c r="V1455" s="42" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="1456" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54620,7 +54623,7 @@
       <c r="T1458" s="8"/>
       <c r="U1458" s="8"/>
       <c r="V1458" s="42" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="1459" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54658,7 +54661,7 @@
       <c r="T1459" s="8"/>
       <c r="U1459" s="8"/>
       <c r="V1459" s="42" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="1460" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54764,7 +54767,7 @@
       <c r="T1462" s="8"/>
       <c r="U1462" s="8"/>
       <c r="V1462" s="42" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="1463" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54800,7 +54803,7 @@
       <c r="T1463" s="8"/>
       <c r="U1463" s="8"/>
       <c r="V1463" s="42" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="1464" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54900,7 +54903,7 @@
       <c r="T1466" s="8"/>
       <c r="U1466" s="8"/>
       <c r="V1466" s="42" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="1467" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55165,7 +55168,7 @@
       <c r="T1474" s="8"/>
       <c r="U1474" s="8"/>
       <c r="V1474" s="42" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="1475" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55235,7 +55238,7 @@
       <c r="T1476" s="8"/>
       <c r="U1476" s="8"/>
       <c r="V1476" s="42" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="1477" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55435,7 +55438,7 @@
       <c r="T1482" s="8"/>
       <c r="U1482" s="8"/>
       <c r="V1482" s="42" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="1483" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55613,7 +55616,7 @@
       <c r="T1487" s="8"/>
       <c r="U1487" s="8"/>
       <c r="V1487" s="42" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="1488" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55713,7 +55716,7 @@
       <c r="T1490" s="8"/>
       <c r="U1490" s="8"/>
       <c r="V1490" s="42" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="1491" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55972,7 +55975,7 @@
       <c r="T1498" s="8"/>
       <c r="U1498" s="8"/>
       <c r="V1498" s="42" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="1499" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56657,7 +56660,7 @@
       <c r="T1519" s="8"/>
       <c r="U1519" s="8"/>
       <c r="V1519" s="42" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="1520" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56917,7 +56920,7 @@
       <c r="T1527" s="8"/>
       <c r="U1527" s="8"/>
       <c r="V1527" s="42" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="1528" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57172,7 +57175,7 @@
       <c r="T1535" s="8"/>
       <c r="U1535" s="8"/>
       <c r="V1535" s="42" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="1536" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57517,7 +57520,7 @@
       <c r="T1546" s="8"/>
       <c r="U1546" s="8"/>
       <c r="V1546" s="42" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="1547" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57583,7 +57586,7 @@
       <c r="T1548" s="8"/>
       <c r="U1548" s="8"/>
       <c r="V1548" s="42" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="1549" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57927,7 +57930,7 @@
       <c r="T1559" s="8"/>
       <c r="U1559" s="8"/>
       <c r="V1559" s="42" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="1560" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58117,7 +58120,7 @@
       <c r="T1565" s="8"/>
       <c r="U1565" s="8"/>
       <c r="V1565" s="42" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="1566" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58820,13 +58823,13 @@
         <v>189</v>
       </c>
       <c r="N1590" s="42" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="P1590" s="8" t="s">
         <v>63</v>
       </c>
       <c r="V1590" s="42" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="1591" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59807,7 +59810,7 @@
         <v>64</v>
       </c>
       <c r="V1630" s="42" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="1631" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60123,7 +60126,7 @@
         <v>64</v>
       </c>
       <c r="V1643" s="42" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="1644" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60152,7 +60155,7 @@
         <v>64</v>
       </c>
       <c r="V1644" s="42" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="1645" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60277,7 +60280,7 @@
         <v>64</v>
       </c>
       <c r="V1649" s="42" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="1650" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60330,7 +60333,7 @@
         <v>64</v>
       </c>
       <c r="V1651" s="42" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="1652" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60650,7 +60653,7 @@
         <v>64</v>
       </c>
       <c r="V1664" s="42" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="1665" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60823,7 +60826,7 @@
         <v>64</v>
       </c>
       <c r="V1671" s="42" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="1672" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61163,7 +61166,7 @@
         <v>64</v>
       </c>
       <c r="V1684" s="42" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="1685" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61300,7 +61303,7 @@
         <v>64</v>
       </c>
       <c r="V1689" s="42" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="1690" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61676,7 +61679,7 @@
         <v>64</v>
       </c>
       <c r="V1704" s="42" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="1705" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61798,7 +61801,7 @@
         <v>119</v>
       </c>
       <c r="N1709" s="42" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="O1709" s="8" t="s">
         <v>64</v>
@@ -61807,7 +61810,7 @@
         <v>63</v>
       </c>
       <c r="V1709" s="42" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="1710" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61882,7 +61885,7 @@
         <v>64</v>
       </c>
       <c r="V1712" s="42" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="1713" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62007,7 +62010,7 @@
         <v>64</v>
       </c>
       <c r="V1717" s="42" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="1718" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62396,7 +62399,7 @@
         <v>64</v>
       </c>
       <c r="V1733" s="42" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="1734" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62710,7 +62713,7 @@
         <v>64</v>
       </c>
       <c r="V1745" s="42" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="1746" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62739,7 +62742,7 @@
         <v>64</v>
       </c>
       <c r="V1746" s="42" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="1747" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63011,7 +63014,7 @@
         <v>64</v>
       </c>
       <c r="V1757" s="42" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="1758" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63234,7 +63237,7 @@
         <v>64</v>
       </c>
       <c r="V1766" s="42" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="1767" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63287,7 +63290,7 @@
         <v>64</v>
       </c>
       <c r="V1768" s="42" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="1769" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63340,7 +63343,7 @@
         <v>64</v>
       </c>
       <c r="V1770" s="42" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="1771" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63489,7 +63492,7 @@
         <v>64</v>
       </c>
       <c r="V1776" s="42" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="1777" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63590,7 +63593,7 @@
         <v>64</v>
       </c>
       <c r="V1780" s="42" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="1781" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64075,7 +64078,7 @@
         <v>64</v>
       </c>
       <c r="V1800" s="42" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="1801" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64458,7 +64461,7 @@
         <v>64</v>
       </c>
       <c r="V1814" s="42" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="1815" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64628,7 +64631,7 @@
         <v>64</v>
       </c>
       <c r="V1820" s="42" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="1821" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64681,7 +64684,7 @@
         <v>64</v>
       </c>
       <c r="V1822" s="42" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="1823" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64734,7 +64737,7 @@
         <v>64</v>
       </c>
       <c r="V1824" s="42" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="1825" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64862,7 +64865,7 @@
         <v>63</v>
       </c>
       <c r="V1829" s="42" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="1830" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64889,7 +64892,7 @@
         <v>64</v>
       </c>
       <c r="V1830" s="42" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="1831" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64966,7 +64969,7 @@
         <v>64</v>
       </c>
       <c r="V1833" s="42" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="1834" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65115,7 +65118,7 @@
         <v>64</v>
       </c>
       <c r="V1839" s="42" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="1840" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65771,7 +65774,7 @@
         <v>64</v>
       </c>
       <c r="V1865" s="42" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="1866" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66088,7 +66091,7 @@
         <v>64</v>
       </c>
       <c r="V1878" s="42" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1879" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66455,7 +66458,7 @@
         <v>64</v>
       </c>
       <c r="V1892" s="42" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1893" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66785,7 +66788,7 @@
         <v>64</v>
       </c>
       <c r="V1905" s="42" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="1906" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66856,13 +66859,13 @@
         <v>79</v>
       </c>
       <c r="N1908" s="43" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="O1908" s="8" t="s">
         <v>64</v>
       </c>
       <c r="V1908" s="43" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="1909" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67526,7 +67529,7 @@
         <v>64</v>
       </c>
       <c r="V1935" s="42" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="1936" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67675,7 +67678,7 @@
         <v>64</v>
       </c>
       <c r="V1941" s="42" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="1942" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67803,7 +67806,7 @@
         <v>111</v>
       </c>
       <c r="T1946" s="8" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="V1946" s="42"/>
     </row>
@@ -67857,7 +67860,7 @@
         <v>64</v>
       </c>
       <c r="V1948" s="42" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="1949" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67937,7 +67940,7 @@
         <v>64</v>
       </c>
       <c r="V1951" s="42" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="1952" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68065,7 +68068,7 @@
         <v>64</v>
       </c>
       <c r="V1956" s="42" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="1957" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68243,7 +68246,7 @@
         <v>64</v>
       </c>
       <c r="V1963" s="42" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="1964" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68344,7 +68347,7 @@
         <v>64</v>
       </c>
       <c r="V1967" s="42" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="1968" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68520,7 +68523,7 @@
         <v>64</v>
       </c>
       <c r="V1974" s="42" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="1975" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68692,7 +68695,7 @@
         <v>64</v>
       </c>
       <c r="V1981" s="42" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="1982" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68772,7 +68775,7 @@
         <v>111</v>
       </c>
       <c r="T1984" s="8" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="V1984" s="42"/>
     </row>
@@ -68826,7 +68829,7 @@
         <v>64</v>
       </c>
       <c r="V1986" s="42" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="1987" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69076,7 +69079,7 @@
         <v>64</v>
       </c>
       <c r="V1996" s="42" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="1997" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69204,7 +69207,7 @@
         <v>64</v>
       </c>
       <c r="V2001" s="42" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="2002" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69281,7 +69284,7 @@
         <v>64</v>
       </c>
       <c r="V2004" s="42" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="2005" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69382,7 +69385,7 @@
         <v>64</v>
       </c>
       <c r="V2008" s="42" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="2009" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69630,7 +69633,7 @@
         <v>111</v>
       </c>
       <c r="T2018" s="8" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="V2018" s="42"/>
     </row>
@@ -69708,7 +69711,7 @@
         <v>64</v>
       </c>
       <c r="V2021" s="42" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="2022" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69814,7 +69817,7 @@
         <v>64</v>
       </c>
       <c r="V2025" s="42" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="2026" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70286,7 +70289,7 @@
     </row>
     <row r="2045" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2045" s="64" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="H2045" s="49" t="s">
         <v>108</v>
@@ -70711,7 +70714,7 @@
         <v>64</v>
       </c>
       <c r="V2060" s="42" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="2061" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71201,7 +71204,7 @@
         <v>64</v>
       </c>
       <c r="V2080" s="42" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="2081" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71329,7 +71332,7 @@
         <v>66</v>
       </c>
       <c r="V2085" s="42" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="2086" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71358,7 +71361,7 @@
         <v>67</v>
       </c>
       <c r="V2086" s="42" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="2087" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71387,7 +71390,7 @@
         <v>64</v>
       </c>
       <c r="V2087" s="42" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="2088" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71497,7 +71500,7 @@
         <v>64</v>
       </c>
       <c r="V2091" s="42" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="2092" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71664,7 +71667,7 @@
         <v>64</v>
       </c>
       <c r="V2097" s="42" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="2098" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71717,7 +71720,7 @@
         <v>64</v>
       </c>
       <c r="V2099" s="42" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="2100" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71770,7 +71773,7 @@
         <v>64</v>
       </c>
       <c r="V2101" s="42" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="2102" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71799,7 +71802,7 @@
         <v>64</v>
       </c>
       <c r="V2102" s="42" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="2103" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71900,7 +71903,7 @@
         <v>64</v>
       </c>
       <c r="V2106" s="42" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="2107" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72225,7 +72228,7 @@
         <v>64</v>
       </c>
       <c r="V2119" s="42" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="2120" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72392,7 +72395,7 @@
         <v>297</v>
       </c>
       <c r="N2126" s="56" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="O2126" s="8" t="s">
         <v>64</v>
@@ -72401,7 +72404,7 @@
         <v>63</v>
       </c>
       <c r="V2126" s="43" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nmv 04 02 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 6.6 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 6.6 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED3BDC2-75AD-41EA-99CC-055C488DF7EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E35711-499D-4FDC-85FF-AE84F6F500A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5491" uniqueCount="1323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5491" uniqueCount="1324">
   <si>
     <t>Passage</t>
   </si>
@@ -4009,6 +4009,9 @@
   </si>
   <si>
     <t>Aqrddhyaqtaq</t>
+  </si>
+  <si>
+    <t>parya#gnikRutam</t>
   </si>
 </sst>
 </file>
@@ -4751,10 +4754,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A858" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1119" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="S864" sqref="S864"/>
+      <selection pane="bottomLeft" activeCell="V1122" sqref="V1122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -43599,8 +43602,8 @@
         <f t="shared" si="53"/>
         <v>13</v>
       </c>
-      <c r="N1122" s="42" t="s">
-        <v>657</v>
+      <c r="N1122" s="43" t="s">
+        <v>1323</v>
       </c>
       <c r="O1122" s="8" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
nmv 05 02 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 6.6 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 6.6 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E35711-499D-4FDC-85FF-AE84F6F500A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA063FF0-8FFD-44F3-9001-874C959534D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5491" uniqueCount="1324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5490" uniqueCount="1324">
   <si>
     <t>Passage</t>
   </si>
@@ -4754,10 +4754,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1119" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1672" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V1122" sqref="V1122"/>
+      <selection pane="bottomLeft" activeCell="N1682" sqref="N1682"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -61106,11 +61106,9 @@
         <v>92</v>
       </c>
       <c r="N1682" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="O1682" s="8" t="s">
-        <v>65</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="O1682" s="8"/>
       <c r="V1682" s="42"/>
     </row>
     <row r="1683" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">

</xml_diff>